<commit_message>
feat: RDCC-3540 Upload Template Improvements
</commit_message>
<xml_diff>
--- a/src/functionalTest/resources/Staff Data Upload with non idam roles.xlsx
+++ b/src/functionalTest/resources/Staff Data Upload with non idam roles.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_224557/Documents/GitHub/new/rd-caseworker-ref-api/src/functionalTest/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_224557/Documents/GitHub/duplicate/rd-caseworker-ref-api/src/functionalTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27244F06-F3D4-004E-9498-56EC56725C4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6996B7F2-95F3-AE4A-904B-91075B3C83B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19520" activeTab="2" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Guidance" sheetId="11" r:id="rId1"/>
     <sheet name="Terminology" sheetId="12" r:id="rId2"/>
-    <sheet name="Case Worker Data" sheetId="1" r:id="rId3"/>
+    <sheet name="Staff Data" sheetId="1" r:id="rId3"/>
     <sheet name="User Type" sheetId="9" state="hidden" r:id="rId4"/>
     <sheet name="Services" sheetId="7" state="hidden" r:id="rId5"/>
     <sheet name="Base Locations" sheetId="6" state="hidden" r:id="rId6"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1890" uniqueCount="1204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1890" uniqueCount="1212">
   <si>
     <t>Region</t>
   </si>
@@ -3378,30 +3378,6 @@
   </si>
   <si>
     <t>Primary Base Location ID</t>
-  </si>
-  <si>
-    <t>Area of Work2 ID</t>
-  </si>
-  <si>
-    <t>Area of Work1 ID</t>
-  </si>
-  <si>
-    <t>Area of Work3 ID</t>
-  </si>
-  <si>
-    <t>Area of Work4 ID</t>
-  </si>
-  <si>
-    <t>Area of Work5 ID</t>
-  </si>
-  <si>
-    <t>Area of Work6 ID</t>
-  </si>
-  <si>
-    <t>Area of Work7 ID</t>
-  </si>
-  <si>
-    <t>Area of Work8 ID</t>
   </si>
   <si>
     <t>Suspended</t>
@@ -3656,6 +3632,54 @@
   </si>
   <si>
     <t>Task Supervisor</t>
+  </si>
+  <si>
+    <t>Service1 ID</t>
+  </si>
+  <si>
+    <t>Service2</t>
+  </si>
+  <si>
+    <t>Service2 ID</t>
+  </si>
+  <si>
+    <t>Service3</t>
+  </si>
+  <si>
+    <t>Service3 ID</t>
+  </si>
+  <si>
+    <t>Service4</t>
+  </si>
+  <si>
+    <t>Service4 ID</t>
+  </si>
+  <si>
+    <t>Service5</t>
+  </si>
+  <si>
+    <t>Service5 ID</t>
+  </si>
+  <si>
+    <t>Service6</t>
+  </si>
+  <si>
+    <t>Service6 ID</t>
+  </si>
+  <si>
+    <t>Service7</t>
+  </si>
+  <si>
+    <t>Service7 ID</t>
+  </si>
+  <si>
+    <t>Service8</t>
+  </si>
+  <si>
+    <t>Service8 ID</t>
+  </si>
+  <si>
+    <t>Service1</t>
   </si>
 </sst>
 </file>
@@ -4960,7 +4984,7 @@
     <row r="1" spans="1:28" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="30"/>
       <c r="B1" s="31" t="s">
-        <v>1172</v>
+        <v>1164</v>
       </c>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
@@ -5744,7 +5768,7 @@
     <row r="29" spans="1:28" ht="26" x14ac:dyDescent="0.3">
       <c r="A29" s="30"/>
       <c r="B29" s="31" t="s">
-        <v>1173</v>
+        <v>1165</v>
       </c>
       <c r="C29" s="30"/>
       <c r="D29" s="30"/>
@@ -6588,7 +6612,7 @@
     <row r="59" spans="1:28" ht="26" x14ac:dyDescent="0.3">
       <c r="A59" s="30"/>
       <c r="B59" s="31" t="s">
-        <v>1174</v>
+        <v>1166</v>
       </c>
       <c r="C59" s="30"/>
       <c r="D59" s="30"/>
@@ -7466,34 +7490,34 @@
   <sheetData>
     <row r="1" spans="1:2" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="33" t="s">
-        <v>1175</v>
+        <v>1167</v>
       </c>
       <c r="B1" s="33" t="s">
-        <v>1176</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="34" t="s">
-        <v>1177</v>
+        <v>1169</v>
       </c>
       <c r="B2" t="s">
-        <v>1178</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="34" t="s">
-        <v>1179</v>
+        <v>1171</v>
       </c>
       <c r="B3" t="s">
-        <v>1180</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="34" t="s">
-        <v>1181</v>
+        <v>1173</v>
       </c>
       <c r="B4" t="s">
-        <v>1182</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -7501,7 +7525,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>1183</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -7509,15 +7533,15 @@
         <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>1184</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="34" t="s">
-        <v>1185</v>
+        <v>1177</v>
       </c>
       <c r="B7" t="s">
-        <v>1186</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -7525,15 +7549,15 @@
         <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>1187</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="34" t="s">
-        <v>1188</v>
+        <v>1180</v>
       </c>
       <c r="B9" t="s">
-        <v>1189</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="48" x14ac:dyDescent="0.2">
@@ -7541,7 +7565,7 @@
         <v>54</v>
       </c>
       <c r="B10" s="35" t="s">
-        <v>1190</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -7549,7 +7573,7 @@
         <v>410</v>
       </c>
       <c r="B11" t="s">
-        <v>1191</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -7557,7 +7581,7 @@
         <v>411</v>
       </c>
       <c r="B12" t="s">
-        <v>1192</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -7565,7 +7589,7 @@
         <v>57</v>
       </c>
       <c r="B13" t="s">
-        <v>1193</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -7573,7 +7597,7 @@
         <v>58</v>
       </c>
       <c r="B14" t="s">
-        <v>1193</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -7581,7 +7605,7 @@
         <v>59</v>
       </c>
       <c r="B15" t="s">
-        <v>1193</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -7589,7 +7613,7 @@
         <v>60</v>
       </c>
       <c r="B16" t="s">
-        <v>1193</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -7597,7 +7621,7 @@
         <v>61</v>
       </c>
       <c r="B17" t="s">
-        <v>1193</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -7605,7 +7629,7 @@
         <v>62</v>
       </c>
       <c r="B18" t="s">
-        <v>1193</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -7613,7 +7637,7 @@
         <v>63</v>
       </c>
       <c r="B19" t="s">
-        <v>1193</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -7621,7 +7645,7 @@
         <v>64</v>
       </c>
       <c r="B20" t="s">
-        <v>1193</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -7629,15 +7653,15 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>1194</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="34" t="s">
-        <v>1195</v>
+        <v>1187</v>
       </c>
       <c r="B22" t="s">
-        <v>1196</v>
+        <v>1188</v>
       </c>
     </row>
   </sheetData>
@@ -7653,8 +7677,8 @@
   </sheetPr>
   <dimension ref="A1:AF50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AF5" sqref="AF5"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7717,7 +7741,7 @@
         <v>56</v>
       </c>
       <c r="I1" s="26" t="s">
-        <v>1197</v>
+        <v>1189</v>
       </c>
       <c r="J1" s="36" t="s">
         <v>54</v>
@@ -7729,78 +7753,78 @@
         <v>411</v>
       </c>
       <c r="M1" s="38" t="s">
-        <v>57</v>
+        <v>1211</v>
       </c>
       <c r="N1" s="27" t="s">
-        <v>1113</v>
+        <v>1196</v>
       </c>
       <c r="O1" s="36" t="s">
-        <v>58</v>
+        <v>1197</v>
       </c>
       <c r="P1" s="29" t="s">
-        <v>1112</v>
+        <v>1198</v>
       </c>
       <c r="Q1" s="39" t="s">
-        <v>59</v>
+        <v>1199</v>
       </c>
       <c r="R1" s="29" t="s">
-        <v>1114</v>
+        <v>1200</v>
       </c>
       <c r="S1" s="38" t="s">
-        <v>60</v>
+        <v>1201</v>
       </c>
       <c r="T1" s="29" t="s">
-        <v>1115</v>
+        <v>1202</v>
       </c>
       <c r="U1" s="38" t="s">
-        <v>61</v>
+        <v>1203</v>
       </c>
       <c r="V1" s="28" t="s">
-        <v>1116</v>
+        <v>1204</v>
       </c>
       <c r="W1" s="38" t="s">
-        <v>62</v>
+        <v>1205</v>
       </c>
       <c r="X1" s="28" t="s">
-        <v>1117</v>
+        <v>1206</v>
       </c>
       <c r="Y1" s="38" t="s">
-        <v>63</v>
+        <v>1207</v>
       </c>
       <c r="Z1" s="28" t="s">
-        <v>1118</v>
+        <v>1208</v>
       </c>
       <c r="AA1" s="38" t="s">
-        <v>64</v>
+        <v>1209</v>
       </c>
       <c r="AB1" s="28" t="s">
-        <v>1119</v>
+        <v>1210</v>
       </c>
       <c r="AC1" s="38" t="s">
         <v>2</v>
       </c>
       <c r="AD1" s="43" t="s">
-        <v>1120</v>
+        <v>1112</v>
       </c>
       <c r="AE1" s="43" t="s">
-        <v>1202</v>
+        <v>1194</v>
       </c>
       <c r="AF1" s="43" t="s">
-        <v>1203</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" s="41" t="str">
         <f t="shared" ref="A2:B4" ca="1" si="0">CHAR(RANDBETWEEN(65,90))&amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122))</f>
-        <v>Ance</v>
+        <v>Obmd</v>
       </c>
       <c r="B2" s="41" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Agpw</v>
+        <v>Ncng</v>
       </c>
       <c r="C2" s="42" t="str">
         <f ca="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
-        <v>CWR-func-test-user-47277210@justice.gov.uk</v>
+        <v>CWR-func-test-user-4205177350@justice.gov.uk</v>
       </c>
       <c r="D2" s="41" t="s">
         <v>5</v>
@@ -7831,7 +7855,7 @@
       </c>
       <c r="L2" s="41"/>
       <c r="M2" s="41" t="s">
-        <v>1169</v>
+        <v>1161</v>
       </c>
       <c r="N2" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(M2,Services!$A$1:$B$45,2)),"",VLOOKUP(M2,Services!$A$1:$B$45,2))</f>
@@ -7873,13 +7897,13 @@
         <v/>
       </c>
       <c r="AC2" s="41" t="s">
-        <v>1199</v>
+        <v>1191</v>
       </c>
       <c r="AD2" s="41" t="s">
-        <v>1121</v>
+        <v>1113</v>
       </c>
       <c r="AE2" s="41" t="s">
-        <v>1121</v>
+        <v>1113</v>
       </c>
       <c r="AF2" s="41" t="s">
         <v>51</v>
@@ -7888,15 +7912,15 @@
     <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A3" s="41" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Okfr</v>
+        <v>Malx</v>
       </c>
       <c r="B3" s="41" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Xzsb</v>
+        <v>Cwzz</v>
       </c>
       <c r="C3" s="42" t="str">
         <f t="shared" ref="C3:C4" ca="1" si="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
-        <v>CWR-func-test-user-8092131557@justice.gov.uk</v>
+        <v>CWR-func-test-user-2669117760@justice.gov.uk</v>
       </c>
       <c r="D3" s="41" t="s">
         <v>6</v>
@@ -7930,7 +7954,7 @@
         <v/>
       </c>
       <c r="O3" s="41" t="s">
-        <v>1168</v>
+        <v>1160</v>
       </c>
       <c r="P3" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(O3,Services!$A$1:$B$45,2)),"",VLOOKUP(O3,Services!$A$1:$B$45,2))</f>
@@ -7968,7 +7992,7 @@
       </c>
       <c r="AC3" s="41"/>
       <c r="AD3" s="41" t="s">
-        <v>1121</v>
+        <v>1113</v>
       </c>
       <c r="AE3" s="41" t="s">
         <v>51</v>
@@ -7980,15 +8004,15 @@
     <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" s="41" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Gdzc</v>
+        <v>Tcyn</v>
       </c>
       <c r="B4" s="41" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Howx</v>
+        <v>Pdke</v>
       </c>
       <c r="C4" s="42" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>CWR-func-test-user-2592229959@justice.gov.uk</v>
+        <v>CWR-func-test-user-8664597760@justice.gov.uk</v>
       </c>
       <c r="D4" s="41" t="s">
         <v>9</v>
@@ -8034,7 +8058,7 @@
         <v/>
       </c>
       <c r="S4" s="41" t="s">
-        <v>1167</v>
+        <v>1159</v>
       </c>
       <c r="T4" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(S4,Services!$A$1:$B$45,2)),"",VLOOKUP(S4,Services!$A$1:$B$45,2))</f>
@@ -8062,25 +8086,25 @@
       </c>
       <c r="AC4" s="41"/>
       <c r="AD4" s="41" t="s">
-        <v>1121</v>
+        <v>1113</v>
       </c>
       <c r="AE4" s="41" t="s">
         <v>51</v>
       </c>
       <c r="AF4" s="41" t="s">
-        <v>1121</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A5" s="41" t="s">
-        <v>1200</v>
+        <v>1192</v>
       </c>
       <c r="B5" s="41" t="s">
-        <v>1200</v>
+        <v>1192</v>
       </c>
       <c r="C5" s="42" t="str">
         <f ca="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
-        <v>CWR-func-test-user-3271897962@justice.gov.uk</v>
+        <v>CWR-func-test-user-7522407260@justice.gov.uk</v>
       </c>
       <c r="D5" s="41" t="s">
         <v>4</v>
@@ -8113,7 +8137,7 @@
         <v>409</v>
       </c>
       <c r="M5" s="41" t="s">
-        <v>1169</v>
+        <v>1161</v>
       </c>
       <c r="N5" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(M5,Services!$A$1:$B$45,2)),"",VLOOKUP(M5,Services!$A$1:$B$45,2))</f>
@@ -8155,10 +8179,10 @@
         <v/>
       </c>
       <c r="AC5" s="41" t="s">
-        <v>1201</v>
+        <v>1193</v>
       </c>
       <c r="AD5" s="41" t="s">
-        <v>1121</v>
+        <v>1113</v>
       </c>
       <c r="AE5" s="41"/>
       <c r="AF5" s="41"/>
@@ -11163,7 +11187,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1198</v>
+        <v>1190</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -11204,7 +11228,7 @@
         <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>1122</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -11212,47 +11236,47 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>1123</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1167</v>
+        <v>1159</v>
       </c>
       <c r="B3" t="s">
-        <v>1124</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>1168</v>
+        <v>1160</v>
       </c>
       <c r="B4" t="s">
-        <v>1125</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>1169</v>
+        <v>1161</v>
       </c>
       <c r="B5" t="s">
-        <v>1126</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>1170</v>
+        <v>1162</v>
       </c>
       <c r="B6" t="s">
-        <v>1127</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>1171</v>
+        <v>1163</v>
       </c>
       <c r="B7" t="s">
-        <v>1128</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -11260,7 +11284,7 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>1129</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -11268,7 +11292,7 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>1130</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -11276,7 +11300,7 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>1131</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -11284,7 +11308,7 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>1132</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -11292,7 +11316,7 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>1133</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -11300,7 +11324,7 @@
         <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>1134</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -11308,7 +11332,7 @@
         <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>1135</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -11316,7 +11340,7 @@
         <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>1136</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -11324,7 +11348,7 @@
         <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>1137</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -11332,7 +11356,7 @@
         <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>1138</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -11340,7 +11364,7 @@
         <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>1139</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -11348,7 +11372,7 @@
         <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>1140</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -11356,7 +11380,7 @@
         <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>1141</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -11364,7 +11388,7 @@
         <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>1142</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -11372,7 +11396,7 @@
         <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>1143</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -11380,7 +11404,7 @@
         <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>1144</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -11388,7 +11412,7 @@
         <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>1145</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -11396,7 +11420,7 @@
         <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>1146</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -11404,7 +11428,7 @@
         <v>31</v>
       </c>
       <c r="B26" t="s">
-        <v>1147</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -11412,7 +11436,7 @@
         <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>1148</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -11420,7 +11444,7 @@
         <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>1149</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -11428,7 +11452,7 @@
         <v>34</v>
       </c>
       <c r="B29" t="s">
-        <v>1150</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -11436,7 +11460,7 @@
         <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>1151</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -11444,7 +11468,7 @@
         <v>36</v>
       </c>
       <c r="B31" t="s">
-        <v>1152</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -11452,7 +11476,7 @@
         <v>37</v>
       </c>
       <c r="B32" t="s">
-        <v>1153</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -11460,7 +11484,7 @@
         <v>38</v>
       </c>
       <c r="B33" t="s">
-        <v>1154</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -11468,7 +11492,7 @@
         <v>39</v>
       </c>
       <c r="B34" t="s">
-        <v>1155</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -11476,7 +11500,7 @@
         <v>40</v>
       </c>
       <c r="B35" t="s">
-        <v>1156</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -11484,7 +11508,7 @@
         <v>41</v>
       </c>
       <c r="B36" t="s">
-        <v>1157</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -11492,7 +11516,7 @@
         <v>42</v>
       </c>
       <c r="B37" t="s">
-        <v>1158</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -11500,7 +11524,7 @@
         <v>43</v>
       </c>
       <c r="B38" t="s">
-        <v>1159</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -11508,7 +11532,7 @@
         <v>44</v>
       </c>
       <c r="B39" t="s">
-        <v>1160</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -11516,7 +11540,7 @@
         <v>45</v>
       </c>
       <c r="B40" t="s">
-        <v>1161</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -11524,7 +11548,7 @@
         <v>46</v>
       </c>
       <c r="B41" t="s">
-        <v>1162</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -11532,7 +11556,7 @@
         <v>47</v>
       </c>
       <c r="B42" t="s">
-        <v>1163</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -11540,7 +11564,7 @@
         <v>48</v>
       </c>
       <c r="B43" t="s">
-        <v>1164</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
@@ -11548,7 +11572,7 @@
         <v>49</v>
       </c>
       <c r="B44" t="s">
-        <v>1165</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
@@ -11556,7 +11580,7 @@
         <v>50</v>
       </c>
       <c r="B45" t="s">
-        <v>1166</v>
+        <v>1158</v>
       </c>
     </row>
   </sheetData>
@@ -18942,7 +18966,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>1121</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
feat: RDCC-3540 Upload Template Improvements (#373)
</commit_message>
<xml_diff>
--- a/src/functionalTest/resources/Staff Data Upload with non idam roles.xlsx
+++ b/src/functionalTest/resources/Staff Data Upload with non idam roles.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_224557/Documents/GitHub/new/rd-caseworker-ref-api/src/functionalTest/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_224557/Documents/GitHub/duplicate/rd-caseworker-ref-api/src/functionalTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27244F06-F3D4-004E-9498-56EC56725C4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6996B7F2-95F3-AE4A-904B-91075B3C83B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19520" activeTab="2" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Guidance" sheetId="11" r:id="rId1"/>
     <sheet name="Terminology" sheetId="12" r:id="rId2"/>
-    <sheet name="Case Worker Data" sheetId="1" r:id="rId3"/>
+    <sheet name="Staff Data" sheetId="1" r:id="rId3"/>
     <sheet name="User Type" sheetId="9" state="hidden" r:id="rId4"/>
     <sheet name="Services" sheetId="7" state="hidden" r:id="rId5"/>
     <sheet name="Base Locations" sheetId="6" state="hidden" r:id="rId6"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1890" uniqueCount="1204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1890" uniqueCount="1212">
   <si>
     <t>Region</t>
   </si>
@@ -3378,30 +3378,6 @@
   </si>
   <si>
     <t>Primary Base Location ID</t>
-  </si>
-  <si>
-    <t>Area of Work2 ID</t>
-  </si>
-  <si>
-    <t>Area of Work1 ID</t>
-  </si>
-  <si>
-    <t>Area of Work3 ID</t>
-  </si>
-  <si>
-    <t>Area of Work4 ID</t>
-  </si>
-  <si>
-    <t>Area of Work5 ID</t>
-  </si>
-  <si>
-    <t>Area of Work6 ID</t>
-  </si>
-  <si>
-    <t>Area of Work7 ID</t>
-  </si>
-  <si>
-    <t>Area of Work8 ID</t>
   </si>
   <si>
     <t>Suspended</t>
@@ -3656,6 +3632,54 @@
   </si>
   <si>
     <t>Task Supervisor</t>
+  </si>
+  <si>
+    <t>Service1 ID</t>
+  </si>
+  <si>
+    <t>Service2</t>
+  </si>
+  <si>
+    <t>Service2 ID</t>
+  </si>
+  <si>
+    <t>Service3</t>
+  </si>
+  <si>
+    <t>Service3 ID</t>
+  </si>
+  <si>
+    <t>Service4</t>
+  </si>
+  <si>
+    <t>Service4 ID</t>
+  </si>
+  <si>
+    <t>Service5</t>
+  </si>
+  <si>
+    <t>Service5 ID</t>
+  </si>
+  <si>
+    <t>Service6</t>
+  </si>
+  <si>
+    <t>Service6 ID</t>
+  </si>
+  <si>
+    <t>Service7</t>
+  </si>
+  <si>
+    <t>Service7 ID</t>
+  </si>
+  <si>
+    <t>Service8</t>
+  </si>
+  <si>
+    <t>Service8 ID</t>
+  </si>
+  <si>
+    <t>Service1</t>
   </si>
 </sst>
 </file>
@@ -4960,7 +4984,7 @@
     <row r="1" spans="1:28" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="30"/>
       <c r="B1" s="31" t="s">
-        <v>1172</v>
+        <v>1164</v>
       </c>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
@@ -5744,7 +5768,7 @@
     <row r="29" spans="1:28" ht="26" x14ac:dyDescent="0.3">
       <c r="A29" s="30"/>
       <c r="B29" s="31" t="s">
-        <v>1173</v>
+        <v>1165</v>
       </c>
       <c r="C29" s="30"/>
       <c r="D29" s="30"/>
@@ -6588,7 +6612,7 @@
     <row r="59" spans="1:28" ht="26" x14ac:dyDescent="0.3">
       <c r="A59" s="30"/>
       <c r="B59" s="31" t="s">
-        <v>1174</v>
+        <v>1166</v>
       </c>
       <c r="C59" s="30"/>
       <c r="D59" s="30"/>
@@ -7466,34 +7490,34 @@
   <sheetData>
     <row r="1" spans="1:2" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="33" t="s">
-        <v>1175</v>
+        <v>1167</v>
       </c>
       <c r="B1" s="33" t="s">
-        <v>1176</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="34" t="s">
-        <v>1177</v>
+        <v>1169</v>
       </c>
       <c r="B2" t="s">
-        <v>1178</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="34" t="s">
-        <v>1179</v>
+        <v>1171</v>
       </c>
       <c r="B3" t="s">
-        <v>1180</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="34" t="s">
-        <v>1181</v>
+        <v>1173</v>
       </c>
       <c r="B4" t="s">
-        <v>1182</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -7501,7 +7525,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>1183</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -7509,15 +7533,15 @@
         <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>1184</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="34" t="s">
-        <v>1185</v>
+        <v>1177</v>
       </c>
       <c r="B7" t="s">
-        <v>1186</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -7525,15 +7549,15 @@
         <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>1187</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="34" t="s">
-        <v>1188</v>
+        <v>1180</v>
       </c>
       <c r="B9" t="s">
-        <v>1189</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="48" x14ac:dyDescent="0.2">
@@ -7541,7 +7565,7 @@
         <v>54</v>
       </c>
       <c r="B10" s="35" t="s">
-        <v>1190</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -7549,7 +7573,7 @@
         <v>410</v>
       </c>
       <c r="B11" t="s">
-        <v>1191</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -7557,7 +7581,7 @@
         <v>411</v>
       </c>
       <c r="B12" t="s">
-        <v>1192</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -7565,7 +7589,7 @@
         <v>57</v>
       </c>
       <c r="B13" t="s">
-        <v>1193</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -7573,7 +7597,7 @@
         <v>58</v>
       </c>
       <c r="B14" t="s">
-        <v>1193</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -7581,7 +7605,7 @@
         <v>59</v>
       </c>
       <c r="B15" t="s">
-        <v>1193</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -7589,7 +7613,7 @@
         <v>60</v>
       </c>
       <c r="B16" t="s">
-        <v>1193</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -7597,7 +7621,7 @@
         <v>61</v>
       </c>
       <c r="B17" t="s">
-        <v>1193</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -7605,7 +7629,7 @@
         <v>62</v>
       </c>
       <c r="B18" t="s">
-        <v>1193</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -7613,7 +7637,7 @@
         <v>63</v>
       </c>
       <c r="B19" t="s">
-        <v>1193</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -7621,7 +7645,7 @@
         <v>64</v>
       </c>
       <c r="B20" t="s">
-        <v>1193</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -7629,15 +7653,15 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>1194</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="34" t="s">
-        <v>1195</v>
+        <v>1187</v>
       </c>
       <c r="B22" t="s">
-        <v>1196</v>
+        <v>1188</v>
       </c>
     </row>
   </sheetData>
@@ -7653,8 +7677,8 @@
   </sheetPr>
   <dimension ref="A1:AF50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AF5" sqref="AF5"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7717,7 +7741,7 @@
         <v>56</v>
       </c>
       <c r="I1" s="26" t="s">
-        <v>1197</v>
+        <v>1189</v>
       </c>
       <c r="J1" s="36" t="s">
         <v>54</v>
@@ -7729,78 +7753,78 @@
         <v>411</v>
       </c>
       <c r="M1" s="38" t="s">
-        <v>57</v>
+        <v>1211</v>
       </c>
       <c r="N1" s="27" t="s">
-        <v>1113</v>
+        <v>1196</v>
       </c>
       <c r="O1" s="36" t="s">
-        <v>58</v>
+        <v>1197</v>
       </c>
       <c r="P1" s="29" t="s">
-        <v>1112</v>
+        <v>1198</v>
       </c>
       <c r="Q1" s="39" t="s">
-        <v>59</v>
+        <v>1199</v>
       </c>
       <c r="R1" s="29" t="s">
-        <v>1114</v>
+        <v>1200</v>
       </c>
       <c r="S1" s="38" t="s">
-        <v>60</v>
+        <v>1201</v>
       </c>
       <c r="T1" s="29" t="s">
-        <v>1115</v>
+        <v>1202</v>
       </c>
       <c r="U1" s="38" t="s">
-        <v>61</v>
+        <v>1203</v>
       </c>
       <c r="V1" s="28" t="s">
-        <v>1116</v>
+        <v>1204</v>
       </c>
       <c r="W1" s="38" t="s">
-        <v>62</v>
+        <v>1205</v>
       </c>
       <c r="X1" s="28" t="s">
-        <v>1117</v>
+        <v>1206</v>
       </c>
       <c r="Y1" s="38" t="s">
-        <v>63</v>
+        <v>1207</v>
       </c>
       <c r="Z1" s="28" t="s">
-        <v>1118</v>
+        <v>1208</v>
       </c>
       <c r="AA1" s="38" t="s">
-        <v>64</v>
+        <v>1209</v>
       </c>
       <c r="AB1" s="28" t="s">
-        <v>1119</v>
+        <v>1210</v>
       </c>
       <c r="AC1" s="38" t="s">
         <v>2</v>
       </c>
       <c r="AD1" s="43" t="s">
-        <v>1120</v>
+        <v>1112</v>
       </c>
       <c r="AE1" s="43" t="s">
-        <v>1202</v>
+        <v>1194</v>
       </c>
       <c r="AF1" s="43" t="s">
-        <v>1203</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" s="41" t="str">
         <f t="shared" ref="A2:B4" ca="1" si="0">CHAR(RANDBETWEEN(65,90))&amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122))</f>
-        <v>Ance</v>
+        <v>Obmd</v>
       </c>
       <c r="B2" s="41" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Agpw</v>
+        <v>Ncng</v>
       </c>
       <c r="C2" s="42" t="str">
         <f ca="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
-        <v>CWR-func-test-user-47277210@justice.gov.uk</v>
+        <v>CWR-func-test-user-4205177350@justice.gov.uk</v>
       </c>
       <c r="D2" s="41" t="s">
         <v>5</v>
@@ -7831,7 +7855,7 @@
       </c>
       <c r="L2" s="41"/>
       <c r="M2" s="41" t="s">
-        <v>1169</v>
+        <v>1161</v>
       </c>
       <c r="N2" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(M2,Services!$A$1:$B$45,2)),"",VLOOKUP(M2,Services!$A$1:$B$45,2))</f>
@@ -7873,13 +7897,13 @@
         <v/>
       </c>
       <c r="AC2" s="41" t="s">
-        <v>1199</v>
+        <v>1191</v>
       </c>
       <c r="AD2" s="41" t="s">
-        <v>1121</v>
+        <v>1113</v>
       </c>
       <c r="AE2" s="41" t="s">
-        <v>1121</v>
+        <v>1113</v>
       </c>
       <c r="AF2" s="41" t="s">
         <v>51</v>
@@ -7888,15 +7912,15 @@
     <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A3" s="41" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Okfr</v>
+        <v>Malx</v>
       </c>
       <c r="B3" s="41" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Xzsb</v>
+        <v>Cwzz</v>
       </c>
       <c r="C3" s="42" t="str">
         <f t="shared" ref="C3:C4" ca="1" si="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
-        <v>CWR-func-test-user-8092131557@justice.gov.uk</v>
+        <v>CWR-func-test-user-2669117760@justice.gov.uk</v>
       </c>
       <c r="D3" s="41" t="s">
         <v>6</v>
@@ -7930,7 +7954,7 @@
         <v/>
       </c>
       <c r="O3" s="41" t="s">
-        <v>1168</v>
+        <v>1160</v>
       </c>
       <c r="P3" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(O3,Services!$A$1:$B$45,2)),"",VLOOKUP(O3,Services!$A$1:$B$45,2))</f>
@@ -7968,7 +7992,7 @@
       </c>
       <c r="AC3" s="41"/>
       <c r="AD3" s="41" t="s">
-        <v>1121</v>
+        <v>1113</v>
       </c>
       <c r="AE3" s="41" t="s">
         <v>51</v>
@@ -7980,15 +8004,15 @@
     <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" s="41" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Gdzc</v>
+        <v>Tcyn</v>
       </c>
       <c r="B4" s="41" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Howx</v>
+        <v>Pdke</v>
       </c>
       <c r="C4" s="42" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>CWR-func-test-user-2592229959@justice.gov.uk</v>
+        <v>CWR-func-test-user-8664597760@justice.gov.uk</v>
       </c>
       <c r="D4" s="41" t="s">
         <v>9</v>
@@ -8034,7 +8058,7 @@
         <v/>
       </c>
       <c r="S4" s="41" t="s">
-        <v>1167</v>
+        <v>1159</v>
       </c>
       <c r="T4" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(S4,Services!$A$1:$B$45,2)),"",VLOOKUP(S4,Services!$A$1:$B$45,2))</f>
@@ -8062,25 +8086,25 @@
       </c>
       <c r="AC4" s="41"/>
       <c r="AD4" s="41" t="s">
-        <v>1121</v>
+        <v>1113</v>
       </c>
       <c r="AE4" s="41" t="s">
         <v>51</v>
       </c>
       <c r="AF4" s="41" t="s">
-        <v>1121</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A5" s="41" t="s">
-        <v>1200</v>
+        <v>1192</v>
       </c>
       <c r="B5" s="41" t="s">
-        <v>1200</v>
+        <v>1192</v>
       </c>
       <c r="C5" s="42" t="str">
         <f ca="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
-        <v>CWR-func-test-user-3271897962@justice.gov.uk</v>
+        <v>CWR-func-test-user-7522407260@justice.gov.uk</v>
       </c>
       <c r="D5" s="41" t="s">
         <v>4</v>
@@ -8113,7 +8137,7 @@
         <v>409</v>
       </c>
       <c r="M5" s="41" t="s">
-        <v>1169</v>
+        <v>1161</v>
       </c>
       <c r="N5" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(M5,Services!$A$1:$B$45,2)),"",VLOOKUP(M5,Services!$A$1:$B$45,2))</f>
@@ -8155,10 +8179,10 @@
         <v/>
       </c>
       <c r="AC5" s="41" t="s">
-        <v>1201</v>
+        <v>1193</v>
       </c>
       <c r="AD5" s="41" t="s">
-        <v>1121</v>
+        <v>1113</v>
       </c>
       <c r="AE5" s="41"/>
       <c r="AF5" s="41"/>
@@ -11163,7 +11187,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1198</v>
+        <v>1190</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -11204,7 +11228,7 @@
         <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>1122</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -11212,47 +11236,47 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>1123</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1167</v>
+        <v>1159</v>
       </c>
       <c r="B3" t="s">
-        <v>1124</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>1168</v>
+        <v>1160</v>
       </c>
       <c r="B4" t="s">
-        <v>1125</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>1169</v>
+        <v>1161</v>
       </c>
       <c r="B5" t="s">
-        <v>1126</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>1170</v>
+        <v>1162</v>
       </c>
       <c r="B6" t="s">
-        <v>1127</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>1171</v>
+        <v>1163</v>
       </c>
       <c r="B7" t="s">
-        <v>1128</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -11260,7 +11284,7 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>1129</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -11268,7 +11292,7 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>1130</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -11276,7 +11300,7 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>1131</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -11284,7 +11308,7 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>1132</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -11292,7 +11316,7 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>1133</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -11300,7 +11324,7 @@
         <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>1134</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -11308,7 +11332,7 @@
         <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>1135</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -11316,7 +11340,7 @@
         <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>1136</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -11324,7 +11348,7 @@
         <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>1137</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -11332,7 +11356,7 @@
         <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>1138</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -11340,7 +11364,7 @@
         <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>1139</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -11348,7 +11372,7 @@
         <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>1140</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -11356,7 +11380,7 @@
         <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>1141</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -11364,7 +11388,7 @@
         <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>1142</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -11372,7 +11396,7 @@
         <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>1143</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -11380,7 +11404,7 @@
         <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>1144</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -11388,7 +11412,7 @@
         <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>1145</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -11396,7 +11420,7 @@
         <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>1146</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -11404,7 +11428,7 @@
         <v>31</v>
       </c>
       <c r="B26" t="s">
-        <v>1147</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -11412,7 +11436,7 @@
         <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>1148</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -11420,7 +11444,7 @@
         <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>1149</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -11428,7 +11452,7 @@
         <v>34</v>
       </c>
       <c r="B29" t="s">
-        <v>1150</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -11436,7 +11460,7 @@
         <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>1151</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -11444,7 +11468,7 @@
         <v>36</v>
       </c>
       <c r="B31" t="s">
-        <v>1152</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -11452,7 +11476,7 @@
         <v>37</v>
       </c>
       <c r="B32" t="s">
-        <v>1153</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -11460,7 +11484,7 @@
         <v>38</v>
       </c>
       <c r="B33" t="s">
-        <v>1154</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -11468,7 +11492,7 @@
         <v>39</v>
       </c>
       <c r="B34" t="s">
-        <v>1155</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -11476,7 +11500,7 @@
         <v>40</v>
       </c>
       <c r="B35" t="s">
-        <v>1156</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -11484,7 +11508,7 @@
         <v>41</v>
       </c>
       <c r="B36" t="s">
-        <v>1157</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -11492,7 +11516,7 @@
         <v>42</v>
       </c>
       <c r="B37" t="s">
-        <v>1158</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -11500,7 +11524,7 @@
         <v>43</v>
       </c>
       <c r="B38" t="s">
-        <v>1159</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -11508,7 +11532,7 @@
         <v>44</v>
       </c>
       <c r="B39" t="s">
-        <v>1160</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -11516,7 +11540,7 @@
         <v>45</v>
       </c>
       <c r="B40" t="s">
-        <v>1161</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -11524,7 +11548,7 @@
         <v>46</v>
       </c>
       <c r="B41" t="s">
-        <v>1162</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -11532,7 +11556,7 @@
         <v>47</v>
       </c>
       <c r="B42" t="s">
-        <v>1163</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -11540,7 +11564,7 @@
         <v>48</v>
       </c>
       <c r="B43" t="s">
-        <v>1164</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
@@ -11548,7 +11572,7 @@
         <v>49</v>
       </c>
       <c r="B44" t="s">
-        <v>1165</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
@@ -11556,7 +11580,7 @@
         <v>50</v>
       </c>
       <c r="B45" t="s">
-        <v>1166</v>
+        <v>1158</v>
       </c>
     </row>
   </sheetData>
@@ -18942,7 +18966,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>1121</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added with Updated Functional Test
</commit_message>
<xml_diff>
--- a/src/functionalTest/resources/Staff Data Upload with non idam roles.xlsx
+++ b/src/functionalTest/resources/Staff Data Upload with non idam roles.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_224557/Documents/GitHub/duplicate/rd-caseworker-ref-api/src/functionalTest/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_2109032/RDCC4025/rd-caseworker-ref-api/src/functionalTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6996B7F2-95F3-AE4A-904B-91075B3C83B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83AB114-2073-9D42-8C67-D85D8DBA340A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19520" activeTab="2" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19520" activeTab="2" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Guidance" sheetId="11" r:id="rId1"/>
     <sheet name="Terminology" sheetId="12" r:id="rId2"/>
     <sheet name="Staff Data" sheetId="1" r:id="rId3"/>
-    <sheet name="User Type" sheetId="9" state="hidden" r:id="rId4"/>
-    <sheet name="Services" sheetId="7" state="hidden" r:id="rId5"/>
-    <sheet name="Base Locations" sheetId="6" state="hidden" r:id="rId6"/>
-    <sheet name="Region" sheetId="3" state="hidden" r:id="rId7"/>
-    <sheet name="Roles" sheetId="4" state="hidden" r:id="rId8"/>
-    <sheet name="Validations" sheetId="10" state="hidden" r:id="rId9"/>
+    <sheet name="User Type" sheetId="9" r:id="rId4"/>
+    <sheet name="Services" sheetId="7" r:id="rId5"/>
+    <sheet name="Base Locations" sheetId="6" r:id="rId6"/>
+    <sheet name="Region" sheetId="3" r:id="rId7"/>
+    <sheet name="Roles" sheetId="4" r:id="rId8"/>
+    <sheet name="Validations" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -7677,8 +7677,8 @@
   </sheetPr>
   <dimension ref="A1:AF50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7695,24 +7695,24 @@
     <col min="10" max="10" width="15.5" style="40" customWidth="1"/>
     <col min="11" max="11" width="25.5" style="40" customWidth="1"/>
     <col min="12" max="12" width="19.5" style="40" customWidth="1"/>
-    <col min="13" max="13" width="24" style="40" customWidth="1"/>
-    <col min="14" max="14" width="24" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="21.33203125" style="40" customWidth="1"/>
-    <col min="16" max="16" width="21.33203125" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="19.1640625" style="40" customWidth="1"/>
-    <col min="18" max="18" width="19.1640625" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="19.1640625" style="40" customWidth="1"/>
-    <col min="20" max="20" width="19.1640625" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="16" style="40" customWidth="1"/>
-    <col min="22" max="22" width="16" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="14.5" style="40" customWidth="1"/>
-    <col min="24" max="24" width="14.5" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="17.33203125" style="40" customWidth="1"/>
-    <col min="26" max="26" width="17.33203125" hidden="1" customWidth="1"/>
-    <col min="27" max="27" width="14.5" style="40" customWidth="1"/>
-    <col min="28" max="28" width="14.5" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="25.5" style="40" customWidth="1"/>
-    <col min="30" max="30" width="9.1640625" style="40"/>
+    <col min="13" max="13" width="8.83203125" style="40"/>
+    <col min="16" max="16" width="24" style="40" customWidth="1"/>
+    <col min="17" max="17" width="24" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="21.33203125" style="40" customWidth="1"/>
+    <col min="19" max="19" width="21.33203125" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="19.1640625" style="40" customWidth="1"/>
+    <col min="21" max="21" width="19.1640625" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="19.1640625" style="40" customWidth="1"/>
+    <col min="23" max="23" width="19.1640625" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="16" style="40" customWidth="1"/>
+    <col min="25" max="25" width="16" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="14.5" style="40" customWidth="1"/>
+    <col min="27" max="27" width="14.5" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="17.33203125" style="40" customWidth="1"/>
+    <col min="29" max="29" width="17.33203125" hidden="1" customWidth="1"/>
+    <col min="30" max="30" width="14.5" style="40" customWidth="1"/>
+    <col min="31" max="31" width="14.5" hidden="1" customWidth="1"/>
+    <col min="32" max="32" width="25.5" style="40" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="42" customHeight="1" x14ac:dyDescent="0.2">
@@ -7752,79 +7752,79 @@
       <c r="L1" s="37" t="s">
         <v>411</v>
       </c>
-      <c r="M1" s="38" t="s">
+      <c r="M1" s="43" t="s">
+        <v>1112</v>
+      </c>
+      <c r="N1" s="43" t="s">
+        <v>1194</v>
+      </c>
+      <c r="O1" s="43" t="s">
+        <v>1195</v>
+      </c>
+      <c r="P1" s="38" t="s">
         <v>1211</v>
       </c>
-      <c r="N1" s="27" t="s">
+      <c r="Q1" s="27" t="s">
         <v>1196</v>
       </c>
-      <c r="O1" s="36" t="s">
+      <c r="R1" s="36" t="s">
         <v>1197</v>
       </c>
-      <c r="P1" s="29" t="s">
+      <c r="S1" s="29" t="s">
         <v>1198</v>
       </c>
-      <c r="Q1" s="39" t="s">
+      <c r="T1" s="39" t="s">
         <v>1199</v>
       </c>
-      <c r="R1" s="29" t="s">
+      <c r="U1" s="29" t="s">
         <v>1200</v>
       </c>
-      <c r="S1" s="38" t="s">
+      <c r="V1" s="38" t="s">
         <v>1201</v>
       </c>
-      <c r="T1" s="29" t="s">
+      <c r="W1" s="29" t="s">
         <v>1202</v>
       </c>
-      <c r="U1" s="38" t="s">
+      <c r="X1" s="38" t="s">
         <v>1203</v>
       </c>
-      <c r="V1" s="28" t="s">
+      <c r="Y1" s="28" t="s">
         <v>1204</v>
       </c>
-      <c r="W1" s="38" t="s">
+      <c r="Z1" s="38" t="s">
         <v>1205</v>
       </c>
-      <c r="X1" s="28" t="s">
+      <c r="AA1" s="28" t="s">
         <v>1206</v>
       </c>
-      <c r="Y1" s="38" t="s">
+      <c r="AB1" s="38" t="s">
         <v>1207</v>
       </c>
-      <c r="Z1" s="28" t="s">
+      <c r="AC1" s="28" t="s">
         <v>1208</v>
       </c>
-      <c r="AA1" s="38" t="s">
+      <c r="AD1" s="38" t="s">
         <v>1209</v>
       </c>
-      <c r="AB1" s="28" t="s">
+      <c r="AE1" s="28" t="s">
         <v>1210</v>
       </c>
-      <c r="AC1" s="38" t="s">
+      <c r="AF1" s="38" t="s">
         <v>2</v>
-      </c>
-      <c r="AD1" s="43" t="s">
-        <v>1112</v>
-      </c>
-      <c r="AE1" s="43" t="s">
-        <v>1194</v>
-      </c>
-      <c r="AF1" s="43" t="s">
-        <v>1195</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" s="41" t="str">
         <f t="shared" ref="A2:B4" ca="1" si="0">CHAR(RANDBETWEEN(65,90))&amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122))</f>
-        <v>Obmd</v>
+        <v>Amwj</v>
       </c>
       <c r="B2" s="41" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Ncng</v>
+        <v>Bpol</v>
       </c>
       <c r="C2" s="42" t="str">
         <f ca="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
-        <v>CWR-func-test-user-4205177350@justice.gov.uk</v>
+        <v>CWR-func-test-user-2960309371@justice.gov.uk</v>
       </c>
       <c r="D2" s="41" t="s">
         <v>5</v>
@@ -7855,72 +7855,72 @@
       </c>
       <c r="L2" s="41"/>
       <c r="M2" s="41" t="s">
+        <v>1113</v>
+      </c>
+      <c r="N2" s="41" t="s">
+        <v>1113</v>
+      </c>
+      <c r="O2" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="P2" s="41" t="s">
         <v>1161</v>
       </c>
-      <c r="N2" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M2,Services!$A$1:$B$45,2)),"",VLOOKUP(M2,Services!$A$1:$B$45,2))</f>
+      <c r="Q2" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P2,Services!$A$1:$B$45,2)),"",VLOOKUP(P2,Services!$A$1:$B$45,2))</f>
         <v>BHA3</v>
       </c>
-      <c r="O2" s="41"/>
-      <c r="P2" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O2,Services!$A$1:$B$45,2)),"",VLOOKUP(O2,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q2" s="41"/>
-      <c r="R2" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q2,Services!$A$1:$B$45,2)),"",VLOOKUP(Q2,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S2" s="41"/>
-      <c r="T2" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S2,Services!$A$1:$B$45,2)),"",VLOOKUP(S2,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U2" s="41"/>
-      <c r="V2" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U2,Services!$A$1:$B$45,2)),"",VLOOKUP(U2,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W2" s="41"/>
-      <c r="X2" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W2,Services!$A$1:$B$45,2)),"",VLOOKUP(W2,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y2" s="41"/>
-      <c r="Z2" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y2,Services!$A$1:$B$45,2)),"",VLOOKUP(Y2,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA2" s="41"/>
-      <c r="AB2" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA2,Services!$A$1:$B$45,2)),"",VLOOKUP(AA2,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC2" s="41" t="s">
+      <c r="R2" s="41"/>
+      <c r="S2" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R2,Services!$A$1:$B$45,2)),"",VLOOKUP(R2,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T2" s="41"/>
+      <c r="U2" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T2,Services!$A$1:$B$45,2)),"",VLOOKUP(T2,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V2" s="41"/>
+      <c r="W2" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V2,Services!$A$1:$B$45,2)),"",VLOOKUP(V2,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X2" s="41"/>
+      <c r="Y2" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X2,Services!$A$1:$B$45,2)),"",VLOOKUP(X2,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z2" s="41"/>
+      <c r="AA2" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z2,Services!$A$1:$B$45,2)),"",VLOOKUP(Z2,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB2" s="41"/>
+      <c r="AC2" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB2,Services!$A$1:$B$45,2)),"",VLOOKUP(AB2,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AD2" s="41"/>
+      <c r="AE2" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD2,Services!$A$1:$B$45,2)),"",VLOOKUP(AD2,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF2" s="41" t="s">
         <v>1191</v>
-      </c>
-      <c r="AD2" s="41" t="s">
-        <v>1113</v>
-      </c>
-      <c r="AE2" s="41" t="s">
-        <v>1113</v>
-      </c>
-      <c r="AF2" s="41" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A3" s="41" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Malx</v>
+        <v>Ycbf</v>
       </c>
       <c r="B3" s="41" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Cwzz</v>
+        <v>Ijej</v>
       </c>
       <c r="C3" s="42" t="str">
         <f t="shared" ref="C3:C4" ca="1" si="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
-        <v>CWR-func-test-user-2669117760@justice.gov.uk</v>
+        <v>CWR-func-test-user-9466180198@justice.gov.uk</v>
       </c>
       <c r="D3" s="41" t="s">
         <v>6</v>
@@ -7948,71 +7948,71 @@
       <c r="L3" s="41" t="s">
         <v>409</v>
       </c>
-      <c r="M3" s="41"/>
-      <c r="N3" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M3,Services!$A$1:$B$45,2)),"",VLOOKUP(M3,Services!$A$1:$B$45,2))</f>
-        <v/>
+      <c r="M3" s="41" t="s">
+        <v>1113</v>
+      </c>
+      <c r="N3" s="41" t="s">
+        <v>51</v>
       </c>
       <c r="O3" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="P3" s="41"/>
+      <c r="Q3" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P3,Services!$A$1:$B$45,2)),"",VLOOKUP(P3,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R3" s="41" t="s">
         <v>1160</v>
       </c>
-      <c r="P3" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O3,Services!$A$1:$B$45,2)),"",VLOOKUP(O3,Services!$A$1:$B$45,2))</f>
+      <c r="S3" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R3,Services!$A$1:$B$45,2)),"",VLOOKUP(R3,Services!$A$1:$B$45,2))</f>
         <v>BAB2</v>
       </c>
-      <c r="Q3" s="41"/>
-      <c r="R3" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q3,Services!$A$1:$B$45,2)),"",VLOOKUP(Q3,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S3" s="41"/>
-      <c r="T3" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S3,Services!$A$1:$B$45,2)),"",VLOOKUP(S3,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U3" s="41"/>
-      <c r="V3" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U3,Services!$A$1:$B$45,2)),"",VLOOKUP(U3,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W3" s="41"/>
-      <c r="X3" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W3,Services!$A$1:$B$45,2)),"",VLOOKUP(W3,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y3" s="41"/>
-      <c r="Z3" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y3,Services!$A$1:$B$45,2)),"",VLOOKUP(Y3,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA3" s="41"/>
-      <c r="AB3" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA3,Services!$A$1:$B$45,2)),"",VLOOKUP(AA3,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC3" s="41"/>
-      <c r="AD3" s="41" t="s">
-        <v>1113</v>
-      </c>
-      <c r="AE3" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="AF3" s="41" t="s">
-        <v>51</v>
-      </c>
+      <c r="T3" s="41"/>
+      <c r="U3" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T3,Services!$A$1:$B$45,2)),"",VLOOKUP(T3,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V3" s="41"/>
+      <c r="W3" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V3,Services!$A$1:$B$45,2)),"",VLOOKUP(V3,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X3" s="41"/>
+      <c r="Y3" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X3,Services!$A$1:$B$45,2)),"",VLOOKUP(X3,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z3" s="41"/>
+      <c r="AA3" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z3,Services!$A$1:$B$45,2)),"",VLOOKUP(Z3,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB3" s="41"/>
+      <c r="AC3" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB3,Services!$A$1:$B$45,2)),"",VLOOKUP(AB3,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AD3" s="41"/>
+      <c r="AE3" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD3,Services!$A$1:$B$45,2)),"",VLOOKUP(AD3,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF3" s="41"/>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" s="41" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Tcyn</v>
+        <v>Onax</v>
       </c>
       <c r="B4" s="41" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Pdke</v>
+        <v>Zvyb</v>
       </c>
       <c r="C4" s="42" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>CWR-func-test-user-8664597760@justice.gov.uk</v>
+        <v>CWR-func-test-user-1300719135@justice.gov.uk</v>
       </c>
       <c r="D4" s="41" t="s">
         <v>9</v>
@@ -8042,58 +8042,58 @@
         <v>408</v>
       </c>
       <c r="L4" s="41"/>
-      <c r="M4" s="41"/>
-      <c r="N4" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M4,Services!$A$1:$B$45,2)),"",VLOOKUP(M4,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O4" s="41"/>
-      <c r="P4" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O4,Services!$A$1:$B$45,2)),"",VLOOKUP(O4,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q4" s="41"/>
-      <c r="R4" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q4,Services!$A$1:$B$45,2)),"",VLOOKUP(Q4,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S4" s="41" t="s">
+      <c r="M4" s="41" t="s">
+        <v>1113</v>
+      </c>
+      <c r="N4" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="O4" s="41" t="s">
+        <v>1113</v>
+      </c>
+      <c r="P4" s="41"/>
+      <c r="Q4" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P4,Services!$A$1:$B$45,2)),"",VLOOKUP(P4,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R4" s="41"/>
+      <c r="S4" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R4,Services!$A$1:$B$45,2)),"",VLOOKUP(R4,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T4" s="41"/>
+      <c r="U4" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T4,Services!$A$1:$B$45,2)),"",VLOOKUP(T4,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V4" s="41" t="s">
         <v>1159</v>
       </c>
-      <c r="T4" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S4,Services!$A$1:$B$45,2)),"",VLOOKUP(S4,Services!$A$1:$B$45,2))</f>
+      <c r="W4" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V4,Services!$A$1:$B$45,2)),"",VLOOKUP(V4,Services!$A$1:$B$45,2))</f>
         <v>BAB2</v>
       </c>
-      <c r="U4" s="41"/>
-      <c r="V4" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U4,Services!$A$1:$B$45,2)),"",VLOOKUP(U4,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W4" s="41"/>
-      <c r="X4" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W4,Services!$A$1:$B$45,2)),"",VLOOKUP(W4,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y4" s="41"/>
-      <c r="Z4" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y4,Services!$A$1:$B$45,2)),"",VLOOKUP(Y4,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA4" s="41"/>
-      <c r="AB4" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA4,Services!$A$1:$B$45,2)),"",VLOOKUP(AA4,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC4" s="41"/>
-      <c r="AD4" s="41" t="s">
-        <v>1113</v>
-      </c>
-      <c r="AE4" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="AF4" s="41" t="s">
-        <v>1113</v>
-      </c>
+      <c r="X4" s="41"/>
+      <c r="Y4" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X4,Services!$A$1:$B$45,2)),"",VLOOKUP(X4,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z4" s="41"/>
+      <c r="AA4" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z4,Services!$A$1:$B$45,2)),"",VLOOKUP(Z4,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB4" s="41"/>
+      <c r="AC4" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB4,Services!$A$1:$B$45,2)),"",VLOOKUP(AB4,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AD4" s="41"/>
+      <c r="AE4" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD4,Services!$A$1:$B$45,2)),"",VLOOKUP(AD4,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF4" s="41"/>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A5" s="41" t="s">
@@ -8104,7 +8104,7 @@
       </c>
       <c r="C5" s="42" t="str">
         <f ca="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
-        <v>CWR-func-test-user-7522407260@justice.gov.uk</v>
+        <v>CWR-func-test-user-3815393503@justice.gov.uk</v>
       </c>
       <c r="D5" s="41" t="s">
         <v>4</v>
@@ -8137,55 +8137,55 @@
         <v>409</v>
       </c>
       <c r="M5" s="41" t="s">
+        <v>1113</v>
+      </c>
+      <c r="N5" s="41"/>
+      <c r="O5" s="41"/>
+      <c r="P5" s="41" t="s">
         <v>1161</v>
       </c>
-      <c r="N5" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M5,Services!$A$1:$B$45,2)),"",VLOOKUP(M5,Services!$A$1:$B$45,2))</f>
+      <c r="Q5" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P5,Services!$A$1:$B$45,2)),"",VLOOKUP(P5,Services!$A$1:$B$45,2))</f>
         <v>BHA3</v>
       </c>
-      <c r="O5" s="41"/>
-      <c r="P5" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O5,Services!$A$1:$B$45,2)),"",VLOOKUP(O5,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q5" s="41"/>
-      <c r="R5" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q5,Services!$A$1:$B$45,2)),"",VLOOKUP(Q5,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S5" s="41"/>
-      <c r="T5" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S5,Services!$A$1:$B$45,2)),"",VLOOKUP(S5,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U5" s="41"/>
-      <c r="V5" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U5,Services!$A$1:$B$45,2)),"",VLOOKUP(U5,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W5" s="41"/>
-      <c r="X5" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W5,Services!$A$1:$B$45,2)),"",VLOOKUP(W5,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y5" s="41"/>
-      <c r="Z5" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y5,Services!$A$1:$B$45,2)),"",VLOOKUP(Y5,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA5" s="41"/>
-      <c r="AB5" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA5,Services!$A$1:$B$45,2)),"",VLOOKUP(AA5,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC5" s="41" t="s">
+      <c r="R5" s="41"/>
+      <c r="S5" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R5,Services!$A$1:$B$45,2)),"",VLOOKUP(R5,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T5" s="41"/>
+      <c r="U5" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T5,Services!$A$1:$B$45,2)),"",VLOOKUP(T5,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V5" s="41"/>
+      <c r="W5" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V5,Services!$A$1:$B$45,2)),"",VLOOKUP(V5,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X5" s="41"/>
+      <c r="Y5" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X5,Services!$A$1:$B$45,2)),"",VLOOKUP(X5,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z5" s="41"/>
+      <c r="AA5" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z5,Services!$A$1:$B$45,2)),"",VLOOKUP(Z5,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB5" s="41"/>
+      <c r="AC5" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB5,Services!$A$1:$B$45,2)),"",VLOOKUP(AB5,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AD5" s="41"/>
+      <c r="AE5" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD5,Services!$A$1:$B$45,2)),"",VLOOKUP(AD5,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF5" s="41" t="s">
         <v>1193</v>
       </c>
-      <c r="AD5" s="41" t="s">
-        <v>1113</v>
-      </c>
-      <c r="AE5" s="41"/>
-      <c r="AF5" s="41"/>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A6" s="41"/>
@@ -8210,47 +8210,49 @@
       <c r="K6" s="41"/>
       <c r="L6" s="41"/>
       <c r="M6" s="41"/>
-      <c r="N6" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M6,Services!$A$1:$B$45,2)),"",VLOOKUP(M6,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O6" s="41"/>
-      <c r="P6" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O6,Services!$A$1:$B$45,2)),"",VLOOKUP(O6,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q6" s="41"/>
-      <c r="R6" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q6,Services!$A$1:$B$45,2)),"",VLOOKUP(Q6,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S6" s="41"/>
-      <c r="T6" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S6,Services!$A$1:$B$45,2)),"",VLOOKUP(S6,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U6" s="41"/>
-      <c r="V6" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U6,Services!$A$1:$B$45,2)),"",VLOOKUP(U6,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W6" s="41"/>
-      <c r="X6" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W6,Services!$A$1:$B$45,2)),"",VLOOKUP(W6,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y6" s="41"/>
-      <c r="Z6" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y6,Services!$A$1:$B$45,2)),"",VLOOKUP(Y6,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA6" s="41"/>
-      <c r="AB6" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA6,Services!$A$1:$B$45,2)),"",VLOOKUP(AA6,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC6" s="41"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="41"/>
+      <c r="Q6" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P6,Services!$A$1:$B$45,2)),"",VLOOKUP(P6,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R6" s="41"/>
+      <c r="S6" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R6,Services!$A$1:$B$45,2)),"",VLOOKUP(R6,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T6" s="41"/>
+      <c r="U6" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T6,Services!$A$1:$B$45,2)),"",VLOOKUP(T6,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V6" s="41"/>
+      <c r="W6" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V6,Services!$A$1:$B$45,2)),"",VLOOKUP(V6,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X6" s="41"/>
+      <c r="Y6" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X6,Services!$A$1:$B$45,2)),"",VLOOKUP(X6,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z6" s="41"/>
+      <c r="AA6" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z6,Services!$A$1:$B$45,2)),"",VLOOKUP(Z6,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB6" s="41"/>
+      <c r="AC6" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB6,Services!$A$1:$B$45,2)),"",VLOOKUP(AB6,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD6" s="41"/>
+      <c r="AE6" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD6,Services!$A$1:$B$45,2)),"",VLOOKUP(AD6,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF6" s="41"/>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A7" s="41"/>
@@ -8275,47 +8277,49 @@
       <c r="K7" s="41"/>
       <c r="L7" s="41"/>
       <c r="M7" s="41"/>
-      <c r="N7" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M7,Services!$A$1:$B$45,2)),"",VLOOKUP(M7,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O7" s="41"/>
-      <c r="P7" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O7,Services!$A$1:$B$45,2)),"",VLOOKUP(O7,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q7" s="41"/>
-      <c r="R7" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q7,Services!$A$1:$B$45,2)),"",VLOOKUP(Q7,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S7" s="41"/>
-      <c r="T7" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S7,Services!$A$1:$B$45,2)),"",VLOOKUP(S7,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U7" s="41"/>
-      <c r="V7" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U7,Services!$A$1:$B$45,2)),"",VLOOKUP(U7,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W7" s="41"/>
-      <c r="X7" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W7,Services!$A$1:$B$45,2)),"",VLOOKUP(W7,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y7" s="41"/>
-      <c r="Z7" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y7,Services!$A$1:$B$45,2)),"",VLOOKUP(Y7,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA7" s="41"/>
-      <c r="AB7" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA7,Services!$A$1:$B$45,2)),"",VLOOKUP(AA7,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC7" s="41"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="41"/>
+      <c r="Q7" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P7,Services!$A$1:$B$45,2)),"",VLOOKUP(P7,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R7" s="41"/>
+      <c r="S7" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R7,Services!$A$1:$B$45,2)),"",VLOOKUP(R7,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T7" s="41"/>
+      <c r="U7" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T7,Services!$A$1:$B$45,2)),"",VLOOKUP(T7,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V7" s="41"/>
+      <c r="W7" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V7,Services!$A$1:$B$45,2)),"",VLOOKUP(V7,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X7" s="41"/>
+      <c r="Y7" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X7,Services!$A$1:$B$45,2)),"",VLOOKUP(X7,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z7" s="41"/>
+      <c r="AA7" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z7,Services!$A$1:$B$45,2)),"",VLOOKUP(Z7,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB7" s="41"/>
+      <c r="AC7" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB7,Services!$A$1:$B$45,2)),"",VLOOKUP(AB7,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD7" s="41"/>
+      <c r="AE7" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD7,Services!$A$1:$B$45,2)),"",VLOOKUP(AD7,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF7" s="41"/>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A8" s="41"/>
@@ -8340,47 +8344,49 @@
       <c r="K8" s="41"/>
       <c r="L8" s="41"/>
       <c r="M8" s="41"/>
-      <c r="N8" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M8,Services!$A$1:$B$45,2)),"",VLOOKUP(M8,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O8" s="41"/>
-      <c r="P8" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O8,Services!$A$1:$B$45,2)),"",VLOOKUP(O8,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q8" s="41"/>
-      <c r="R8" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q8,Services!$A$1:$B$45,2)),"",VLOOKUP(Q8,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S8" s="41"/>
-      <c r="T8" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S8,Services!$A$1:$B$45,2)),"",VLOOKUP(S8,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U8" s="41"/>
-      <c r="V8" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U8,Services!$A$1:$B$45,2)),"",VLOOKUP(U8,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W8" s="41"/>
-      <c r="X8" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W8,Services!$A$1:$B$45,2)),"",VLOOKUP(W8,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y8" s="41"/>
-      <c r="Z8" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y8,Services!$A$1:$B$45,2)),"",VLOOKUP(Y8,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA8" s="41"/>
-      <c r="AB8" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA8,Services!$A$1:$B$45,2)),"",VLOOKUP(AA8,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC8" s="41"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="41"/>
+      <c r="Q8" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P8,Services!$A$1:$B$45,2)),"",VLOOKUP(P8,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R8" s="41"/>
+      <c r="S8" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R8,Services!$A$1:$B$45,2)),"",VLOOKUP(R8,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T8" s="41"/>
+      <c r="U8" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T8,Services!$A$1:$B$45,2)),"",VLOOKUP(T8,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V8" s="41"/>
+      <c r="W8" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V8,Services!$A$1:$B$45,2)),"",VLOOKUP(V8,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X8" s="41"/>
+      <c r="Y8" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X8,Services!$A$1:$B$45,2)),"",VLOOKUP(X8,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z8" s="41"/>
+      <c r="AA8" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z8,Services!$A$1:$B$45,2)),"",VLOOKUP(Z8,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB8" s="41"/>
+      <c r="AC8" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB8,Services!$A$1:$B$45,2)),"",VLOOKUP(AB8,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD8" s="41"/>
+      <c r="AE8" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD8,Services!$A$1:$B$45,2)),"",VLOOKUP(AD8,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF8" s="41"/>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A9" s="41"/>
@@ -8405,47 +8411,49 @@
       <c r="K9" s="41"/>
       <c r="L9" s="41"/>
       <c r="M9" s="41"/>
-      <c r="N9" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M9,Services!$A$1:$B$45,2)),"",VLOOKUP(M9,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O9" s="41"/>
-      <c r="P9" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O9,Services!$A$1:$B$45,2)),"",VLOOKUP(O9,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q9" s="41"/>
-      <c r="R9" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q9,Services!$A$1:$B$45,2)),"",VLOOKUP(Q9,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S9" s="41"/>
-      <c r="T9" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S9,Services!$A$1:$B$45,2)),"",VLOOKUP(S9,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U9" s="41"/>
-      <c r="V9" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U9,Services!$A$1:$B$45,2)),"",VLOOKUP(U9,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W9" s="41"/>
-      <c r="X9" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W9,Services!$A$1:$B$45,2)),"",VLOOKUP(W9,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y9" s="41"/>
-      <c r="Z9" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y9,Services!$A$1:$B$45,2)),"",VLOOKUP(Y9,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA9" s="41"/>
-      <c r="AB9" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA9,Services!$A$1:$B$45,2)),"",VLOOKUP(AA9,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC9" s="41"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="41"/>
+      <c r="Q9" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P9,Services!$A$1:$B$45,2)),"",VLOOKUP(P9,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R9" s="41"/>
+      <c r="S9" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R9,Services!$A$1:$B$45,2)),"",VLOOKUP(R9,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T9" s="41"/>
+      <c r="U9" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T9,Services!$A$1:$B$45,2)),"",VLOOKUP(T9,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V9" s="41"/>
+      <c r="W9" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V9,Services!$A$1:$B$45,2)),"",VLOOKUP(V9,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X9" s="41"/>
+      <c r="Y9" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X9,Services!$A$1:$B$45,2)),"",VLOOKUP(X9,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z9" s="41"/>
+      <c r="AA9" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z9,Services!$A$1:$B$45,2)),"",VLOOKUP(Z9,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB9" s="41"/>
+      <c r="AC9" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB9,Services!$A$1:$B$45,2)),"",VLOOKUP(AB9,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD9" s="41"/>
+      <c r="AE9" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD9,Services!$A$1:$B$45,2)),"",VLOOKUP(AD9,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF9" s="41"/>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A10" s="41"/>
@@ -8470,47 +8478,49 @@
       <c r="K10" s="41"/>
       <c r="L10" s="41"/>
       <c r="M10" s="41"/>
-      <c r="N10" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M10,Services!$A$1:$B$45,2)),"",VLOOKUP(M10,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O10" s="41"/>
-      <c r="P10" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O10,Services!$A$1:$B$45,2)),"",VLOOKUP(O10,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q10" s="41"/>
-      <c r="R10" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q10,Services!$A$1:$B$45,2)),"",VLOOKUP(Q10,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S10" s="41"/>
-      <c r="T10" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S10,Services!$A$1:$B$45,2)),"",VLOOKUP(S10,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U10" s="41"/>
-      <c r="V10" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U10,Services!$A$1:$B$45,2)),"",VLOOKUP(U10,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W10" s="41"/>
-      <c r="X10" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W10,Services!$A$1:$B$45,2)),"",VLOOKUP(W10,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y10" s="41"/>
-      <c r="Z10" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y10,Services!$A$1:$B$45,2)),"",VLOOKUP(Y10,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA10" s="41"/>
-      <c r="AB10" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA10,Services!$A$1:$B$45,2)),"",VLOOKUP(AA10,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC10" s="41"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="41"/>
+      <c r="Q10" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P10,Services!$A$1:$B$45,2)),"",VLOOKUP(P10,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R10" s="41"/>
+      <c r="S10" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R10,Services!$A$1:$B$45,2)),"",VLOOKUP(R10,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T10" s="41"/>
+      <c r="U10" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T10,Services!$A$1:$B$45,2)),"",VLOOKUP(T10,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V10" s="41"/>
+      <c r="W10" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V10,Services!$A$1:$B$45,2)),"",VLOOKUP(V10,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X10" s="41"/>
+      <c r="Y10" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X10,Services!$A$1:$B$45,2)),"",VLOOKUP(X10,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z10" s="41"/>
+      <c r="AA10" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z10,Services!$A$1:$B$45,2)),"",VLOOKUP(Z10,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB10" s="41"/>
+      <c r="AC10" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB10,Services!$A$1:$B$45,2)),"",VLOOKUP(AB10,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD10" s="41"/>
+      <c r="AE10" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD10,Services!$A$1:$B$45,2)),"",VLOOKUP(AD10,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF10" s="41"/>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A11" s="41"/>
@@ -8535,47 +8545,49 @@
       <c r="K11" s="41"/>
       <c r="L11" s="41"/>
       <c r="M11" s="41"/>
-      <c r="N11" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M11,Services!$A$1:$B$45,2)),"",VLOOKUP(M11,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O11" s="41"/>
-      <c r="P11" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O11,Services!$A$1:$B$45,2)),"",VLOOKUP(O11,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q11" s="41"/>
-      <c r="R11" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q11,Services!$A$1:$B$45,2)),"",VLOOKUP(Q11,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S11" s="41"/>
-      <c r="T11" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S11,Services!$A$1:$B$45,2)),"",VLOOKUP(S11,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U11" s="41"/>
-      <c r="V11" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U11,Services!$A$1:$B$45,2)),"",VLOOKUP(U11,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W11" s="41"/>
-      <c r="X11" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W11,Services!$A$1:$B$45,2)),"",VLOOKUP(W11,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y11" s="41"/>
-      <c r="Z11" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y11,Services!$A$1:$B$45,2)),"",VLOOKUP(Y11,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA11" s="41"/>
-      <c r="AB11" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA11,Services!$A$1:$B$45,2)),"",VLOOKUP(AA11,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC11" s="41"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="41"/>
+      <c r="Q11" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P11,Services!$A$1:$B$45,2)),"",VLOOKUP(P11,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R11" s="41"/>
+      <c r="S11" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R11,Services!$A$1:$B$45,2)),"",VLOOKUP(R11,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T11" s="41"/>
+      <c r="U11" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T11,Services!$A$1:$B$45,2)),"",VLOOKUP(T11,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V11" s="41"/>
+      <c r="W11" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V11,Services!$A$1:$B$45,2)),"",VLOOKUP(V11,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X11" s="41"/>
+      <c r="Y11" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X11,Services!$A$1:$B$45,2)),"",VLOOKUP(X11,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z11" s="41"/>
+      <c r="AA11" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z11,Services!$A$1:$B$45,2)),"",VLOOKUP(Z11,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB11" s="41"/>
+      <c r="AC11" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB11,Services!$A$1:$B$45,2)),"",VLOOKUP(AB11,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD11" s="41"/>
+      <c r="AE11" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD11,Services!$A$1:$B$45,2)),"",VLOOKUP(AD11,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF11" s="41"/>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A12" s="41"/>
@@ -8600,47 +8612,49 @@
       <c r="K12" s="41"/>
       <c r="L12" s="41"/>
       <c r="M12" s="41"/>
-      <c r="N12" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M12,Services!$A$1:$B$45,2)),"",VLOOKUP(M12,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O12" s="41"/>
-      <c r="P12" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O12,Services!$A$1:$B$45,2)),"",VLOOKUP(O12,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q12" s="41"/>
-      <c r="R12" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q12,Services!$A$1:$B$45,2)),"",VLOOKUP(Q12,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S12" s="41"/>
-      <c r="T12" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S12,Services!$A$1:$B$45,2)),"",VLOOKUP(S12,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U12" s="41"/>
-      <c r="V12" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U12,Services!$A$1:$B$45,2)),"",VLOOKUP(U12,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W12" s="41"/>
-      <c r="X12" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W12,Services!$A$1:$B$45,2)),"",VLOOKUP(W12,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y12" s="41"/>
-      <c r="Z12" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y12,Services!$A$1:$B$45,2)),"",VLOOKUP(Y12,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA12" s="41"/>
-      <c r="AB12" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA12,Services!$A$1:$B$45,2)),"",VLOOKUP(AA12,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC12" s="41"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="41"/>
+      <c r="Q12" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P12,Services!$A$1:$B$45,2)),"",VLOOKUP(P12,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R12" s="41"/>
+      <c r="S12" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R12,Services!$A$1:$B$45,2)),"",VLOOKUP(R12,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T12" s="41"/>
+      <c r="U12" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T12,Services!$A$1:$B$45,2)),"",VLOOKUP(T12,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V12" s="41"/>
+      <c r="W12" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V12,Services!$A$1:$B$45,2)),"",VLOOKUP(V12,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X12" s="41"/>
+      <c r="Y12" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X12,Services!$A$1:$B$45,2)),"",VLOOKUP(X12,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z12" s="41"/>
+      <c r="AA12" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z12,Services!$A$1:$B$45,2)),"",VLOOKUP(Z12,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB12" s="41"/>
+      <c r="AC12" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB12,Services!$A$1:$B$45,2)),"",VLOOKUP(AB12,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD12" s="41"/>
+      <c r="AE12" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD12,Services!$A$1:$B$45,2)),"",VLOOKUP(AD12,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF12" s="41"/>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A13" s="41"/>
@@ -8665,47 +8679,49 @@
       <c r="K13" s="41"/>
       <c r="L13" s="41"/>
       <c r="M13" s="41"/>
-      <c r="N13" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M13,Services!$A$1:$B$45,2)),"",VLOOKUP(M13,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O13" s="41"/>
-      <c r="P13" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O13,Services!$A$1:$B$45,2)),"",VLOOKUP(O13,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q13" s="41"/>
-      <c r="R13" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q13,Services!$A$1:$B$45,2)),"",VLOOKUP(Q13,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S13" s="41"/>
-      <c r="T13" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S13,Services!$A$1:$B$45,2)),"",VLOOKUP(S13,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U13" s="41"/>
-      <c r="V13" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U13,Services!$A$1:$B$45,2)),"",VLOOKUP(U13,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W13" s="41"/>
-      <c r="X13" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W13,Services!$A$1:$B$45,2)),"",VLOOKUP(W13,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y13" s="41"/>
-      <c r="Z13" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y13,Services!$A$1:$B$45,2)),"",VLOOKUP(Y13,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA13" s="41"/>
-      <c r="AB13" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA13,Services!$A$1:$B$45,2)),"",VLOOKUP(AA13,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC13" s="41"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="41"/>
+      <c r="Q13" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P13,Services!$A$1:$B$45,2)),"",VLOOKUP(P13,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R13" s="41"/>
+      <c r="S13" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R13,Services!$A$1:$B$45,2)),"",VLOOKUP(R13,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T13" s="41"/>
+      <c r="U13" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T13,Services!$A$1:$B$45,2)),"",VLOOKUP(T13,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V13" s="41"/>
+      <c r="W13" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V13,Services!$A$1:$B$45,2)),"",VLOOKUP(V13,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X13" s="41"/>
+      <c r="Y13" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X13,Services!$A$1:$B$45,2)),"",VLOOKUP(X13,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z13" s="41"/>
+      <c r="AA13" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z13,Services!$A$1:$B$45,2)),"",VLOOKUP(Z13,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB13" s="41"/>
+      <c r="AC13" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB13,Services!$A$1:$B$45,2)),"",VLOOKUP(AB13,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD13" s="41"/>
+      <c r="AE13" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD13,Services!$A$1:$B$45,2)),"",VLOOKUP(AD13,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF13" s="41"/>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A14" s="41"/>
@@ -8730,47 +8746,49 @@
       <c r="K14" s="41"/>
       <c r="L14" s="41"/>
       <c r="M14" s="41"/>
-      <c r="N14" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M14,Services!$A$1:$B$45,2)),"",VLOOKUP(M14,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O14" s="41"/>
-      <c r="P14" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O14,Services!$A$1:$B$45,2)),"",VLOOKUP(O14,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q14" s="41"/>
-      <c r="R14" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q14,Services!$A$1:$B$45,2)),"",VLOOKUP(Q14,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S14" s="41"/>
-      <c r="T14" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S14,Services!$A$1:$B$45,2)),"",VLOOKUP(S14,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U14" s="41"/>
-      <c r="V14" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U14,Services!$A$1:$B$45,2)),"",VLOOKUP(U14,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W14" s="41"/>
-      <c r="X14" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W14,Services!$A$1:$B$45,2)),"",VLOOKUP(W14,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y14" s="41"/>
-      <c r="Z14" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y14,Services!$A$1:$B$45,2)),"",VLOOKUP(Y14,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA14" s="41"/>
-      <c r="AB14" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA14,Services!$A$1:$B$45,2)),"",VLOOKUP(AA14,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC14" s="41"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="41"/>
+      <c r="Q14" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P14,Services!$A$1:$B$45,2)),"",VLOOKUP(P14,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R14" s="41"/>
+      <c r="S14" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R14,Services!$A$1:$B$45,2)),"",VLOOKUP(R14,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T14" s="41"/>
+      <c r="U14" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T14,Services!$A$1:$B$45,2)),"",VLOOKUP(T14,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V14" s="41"/>
+      <c r="W14" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V14,Services!$A$1:$B$45,2)),"",VLOOKUP(V14,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X14" s="41"/>
+      <c r="Y14" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X14,Services!$A$1:$B$45,2)),"",VLOOKUP(X14,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z14" s="41"/>
+      <c r="AA14" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z14,Services!$A$1:$B$45,2)),"",VLOOKUP(Z14,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB14" s="41"/>
+      <c r="AC14" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB14,Services!$A$1:$B$45,2)),"",VLOOKUP(AB14,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD14" s="41"/>
+      <c r="AE14" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD14,Services!$A$1:$B$45,2)),"",VLOOKUP(AD14,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF14" s="41"/>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A15" s="41"/>
@@ -8795,47 +8813,49 @@
       <c r="K15" s="41"/>
       <c r="L15" s="41"/>
       <c r="M15" s="41"/>
-      <c r="N15" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M15,Services!$A$1:$B$45,2)),"",VLOOKUP(M15,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O15" s="41"/>
-      <c r="P15" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O15,Services!$A$1:$B$45,2)),"",VLOOKUP(O15,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q15" s="41"/>
-      <c r="R15" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q15,Services!$A$1:$B$45,2)),"",VLOOKUP(Q15,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S15" s="41"/>
-      <c r="T15" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S15,Services!$A$1:$B$45,2)),"",VLOOKUP(S15,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U15" s="41"/>
-      <c r="V15" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U15,Services!$A$1:$B$45,2)),"",VLOOKUP(U15,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W15" s="41"/>
-      <c r="X15" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W15,Services!$A$1:$B$45,2)),"",VLOOKUP(W15,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y15" s="41"/>
-      <c r="Z15" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y15,Services!$A$1:$B$45,2)),"",VLOOKUP(Y15,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA15" s="41"/>
-      <c r="AB15" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA15,Services!$A$1:$B$45,2)),"",VLOOKUP(AA15,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC15" s="41"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="41"/>
+      <c r="Q15" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P15,Services!$A$1:$B$45,2)),"",VLOOKUP(P15,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R15" s="41"/>
+      <c r="S15" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R15,Services!$A$1:$B$45,2)),"",VLOOKUP(R15,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T15" s="41"/>
+      <c r="U15" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T15,Services!$A$1:$B$45,2)),"",VLOOKUP(T15,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V15" s="41"/>
+      <c r="W15" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V15,Services!$A$1:$B$45,2)),"",VLOOKUP(V15,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X15" s="41"/>
+      <c r="Y15" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X15,Services!$A$1:$B$45,2)),"",VLOOKUP(X15,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z15" s="41"/>
+      <c r="AA15" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z15,Services!$A$1:$B$45,2)),"",VLOOKUP(Z15,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB15" s="41"/>
+      <c r="AC15" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB15,Services!$A$1:$B$45,2)),"",VLOOKUP(AB15,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD15" s="41"/>
+      <c r="AE15" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD15,Services!$A$1:$B$45,2)),"",VLOOKUP(AD15,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF15" s="41"/>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A16" s="41"/>
@@ -8860,49 +8880,51 @@
       <c r="K16" s="41"/>
       <c r="L16" s="41"/>
       <c r="M16" s="41"/>
-      <c r="N16" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M16,Services!$A$1:$B$45,2)),"",VLOOKUP(M16,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O16" s="41"/>
-      <c r="P16" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O16,Services!$A$1:$B$45,2)),"",VLOOKUP(O16,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q16" s="41"/>
-      <c r="R16" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q16,Services!$A$1:$B$45,2)),"",VLOOKUP(Q16,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S16" s="41"/>
-      <c r="T16" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S16,Services!$A$1:$B$45,2)),"",VLOOKUP(S16,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U16" s="41"/>
-      <c r="V16" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U16,Services!$A$1:$B$45,2)),"",VLOOKUP(U16,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W16" s="41"/>
-      <c r="X16" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W16,Services!$A$1:$B$45,2)),"",VLOOKUP(W16,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y16" s="41"/>
-      <c r="Z16" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y16,Services!$A$1:$B$45,2)),"",VLOOKUP(Y16,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA16" s="41"/>
-      <c r="AB16" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA16,Services!$A$1:$B$45,2)),"",VLOOKUP(AA16,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC16" s="41"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="41"/>
+      <c r="Q16" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P16,Services!$A$1:$B$45,2)),"",VLOOKUP(P16,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R16" s="41"/>
+      <c r="S16" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R16,Services!$A$1:$B$45,2)),"",VLOOKUP(R16,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T16" s="41"/>
+      <c r="U16" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T16,Services!$A$1:$B$45,2)),"",VLOOKUP(T16,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V16" s="41"/>
+      <c r="W16" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V16,Services!$A$1:$B$45,2)),"",VLOOKUP(V16,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X16" s="41"/>
+      <c r="Y16" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X16,Services!$A$1:$B$45,2)),"",VLOOKUP(X16,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z16" s="41"/>
+      <c r="AA16" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z16,Services!$A$1:$B$45,2)),"",VLOOKUP(Z16,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB16" s="41"/>
+      <c r="AC16" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB16,Services!$A$1:$B$45,2)),"",VLOOKUP(AB16,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD16" s="41"/>
-    </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE16" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD16,Services!$A$1:$B$45,2)),"",VLOOKUP(AD16,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF16" s="41"/>
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A17" s="41"/>
       <c r="B17" s="41"/>
       <c r="C17" s="42"/>
@@ -8925,49 +8947,51 @@
       <c r="K17" s="41"/>
       <c r="L17" s="41"/>
       <c r="M17" s="41"/>
-      <c r="N17" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M17,Services!$A$1:$B$45,2)),"",VLOOKUP(M17,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O17" s="41"/>
-      <c r="P17" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O17,Services!$A$1:$B$45,2)),"",VLOOKUP(O17,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q17" s="41"/>
-      <c r="R17" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q17,Services!$A$1:$B$45,2)),"",VLOOKUP(Q17,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S17" s="41"/>
-      <c r="T17" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S17,Services!$A$1:$B$45,2)),"",VLOOKUP(S17,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U17" s="41"/>
-      <c r="V17" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U17,Services!$A$1:$B$45,2)),"",VLOOKUP(U17,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W17" s="41"/>
-      <c r="X17" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W17,Services!$A$1:$B$45,2)),"",VLOOKUP(W17,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y17" s="41"/>
-      <c r="Z17" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y17,Services!$A$1:$B$45,2)),"",VLOOKUP(Y17,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA17" s="41"/>
-      <c r="AB17" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA17,Services!$A$1:$B$45,2)),"",VLOOKUP(AA17,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC17" s="41"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="41"/>
+      <c r="Q17" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P17,Services!$A$1:$B$45,2)),"",VLOOKUP(P17,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R17" s="41"/>
+      <c r="S17" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R17,Services!$A$1:$B$45,2)),"",VLOOKUP(R17,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T17" s="41"/>
+      <c r="U17" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T17,Services!$A$1:$B$45,2)),"",VLOOKUP(T17,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V17" s="41"/>
+      <c r="W17" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V17,Services!$A$1:$B$45,2)),"",VLOOKUP(V17,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X17" s="41"/>
+      <c r="Y17" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X17,Services!$A$1:$B$45,2)),"",VLOOKUP(X17,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z17" s="41"/>
+      <c r="AA17" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z17,Services!$A$1:$B$45,2)),"",VLOOKUP(Z17,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB17" s="41"/>
+      <c r="AC17" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB17,Services!$A$1:$B$45,2)),"",VLOOKUP(AB17,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD17" s="41"/>
-    </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE17" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD17,Services!$A$1:$B$45,2)),"",VLOOKUP(AD17,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF17" s="41"/>
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A18" s="41"/>
       <c r="B18" s="41"/>
       <c r="C18" s="42"/>
@@ -8990,49 +9014,51 @@
       <c r="K18" s="41"/>
       <c r="L18" s="41"/>
       <c r="M18" s="41"/>
-      <c r="N18" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M18,Services!$A$1:$B$45,2)),"",VLOOKUP(M18,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O18" s="41"/>
-      <c r="P18" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O18,Services!$A$1:$B$45,2)),"",VLOOKUP(O18,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q18" s="41"/>
-      <c r="R18" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q18,Services!$A$1:$B$45,2)),"",VLOOKUP(Q18,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S18" s="41"/>
-      <c r="T18" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S18,Services!$A$1:$B$45,2)),"",VLOOKUP(S18,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U18" s="41"/>
-      <c r="V18" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U18,Services!$A$1:$B$45,2)),"",VLOOKUP(U18,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W18" s="41"/>
-      <c r="X18" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W18,Services!$A$1:$B$45,2)),"",VLOOKUP(W18,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y18" s="41"/>
-      <c r="Z18" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y18,Services!$A$1:$B$45,2)),"",VLOOKUP(Y18,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA18" s="41"/>
-      <c r="AB18" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA18,Services!$A$1:$B$45,2)),"",VLOOKUP(AA18,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC18" s="41"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="41"/>
+      <c r="Q18" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P18,Services!$A$1:$B$45,2)),"",VLOOKUP(P18,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R18" s="41"/>
+      <c r="S18" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R18,Services!$A$1:$B$45,2)),"",VLOOKUP(R18,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T18" s="41"/>
+      <c r="U18" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T18,Services!$A$1:$B$45,2)),"",VLOOKUP(T18,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V18" s="41"/>
+      <c r="W18" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V18,Services!$A$1:$B$45,2)),"",VLOOKUP(V18,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X18" s="41"/>
+      <c r="Y18" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X18,Services!$A$1:$B$45,2)),"",VLOOKUP(X18,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z18" s="41"/>
+      <c r="AA18" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z18,Services!$A$1:$B$45,2)),"",VLOOKUP(Z18,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB18" s="41"/>
+      <c r="AC18" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB18,Services!$A$1:$B$45,2)),"",VLOOKUP(AB18,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD18" s="41"/>
-    </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE18" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD18,Services!$A$1:$B$45,2)),"",VLOOKUP(AD18,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF18" s="41"/>
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A19" s="41"/>
       <c r="B19" s="41"/>
       <c r="C19" s="42"/>
@@ -9055,49 +9081,51 @@
       <c r="K19" s="41"/>
       <c r="L19" s="41"/>
       <c r="M19" s="41"/>
-      <c r="N19" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M19,Services!$A$1:$B$45,2)),"",VLOOKUP(M19,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O19" s="41"/>
-      <c r="P19" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O19,Services!$A$1:$B$45,2)),"",VLOOKUP(O19,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q19" s="41"/>
-      <c r="R19" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q19,Services!$A$1:$B$45,2)),"",VLOOKUP(Q19,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S19" s="41"/>
-      <c r="T19" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S19,Services!$A$1:$B$45,2)),"",VLOOKUP(S19,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U19" s="41"/>
-      <c r="V19" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U19,Services!$A$1:$B$45,2)),"",VLOOKUP(U19,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W19" s="41"/>
-      <c r="X19" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W19,Services!$A$1:$B$45,2)),"",VLOOKUP(W19,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y19" s="41"/>
-      <c r="Z19" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y19,Services!$A$1:$B$45,2)),"",VLOOKUP(Y19,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA19" s="41"/>
-      <c r="AB19" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA19,Services!$A$1:$B$45,2)),"",VLOOKUP(AA19,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC19" s="41"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="41"/>
+      <c r="Q19" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P19,Services!$A$1:$B$45,2)),"",VLOOKUP(P19,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R19" s="41"/>
+      <c r="S19" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R19,Services!$A$1:$B$45,2)),"",VLOOKUP(R19,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T19" s="41"/>
+      <c r="U19" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T19,Services!$A$1:$B$45,2)),"",VLOOKUP(T19,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V19" s="41"/>
+      <c r="W19" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V19,Services!$A$1:$B$45,2)),"",VLOOKUP(V19,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X19" s="41"/>
+      <c r="Y19" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X19,Services!$A$1:$B$45,2)),"",VLOOKUP(X19,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z19" s="41"/>
+      <c r="AA19" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z19,Services!$A$1:$B$45,2)),"",VLOOKUP(Z19,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB19" s="41"/>
+      <c r="AC19" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB19,Services!$A$1:$B$45,2)),"",VLOOKUP(AB19,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD19" s="41"/>
-    </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE19" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD19,Services!$A$1:$B$45,2)),"",VLOOKUP(AD19,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF19" s="41"/>
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A20" s="41"/>
       <c r="B20" s="41"/>
       <c r="C20" s="42"/>
@@ -9120,49 +9148,51 @@
       <c r="K20" s="41"/>
       <c r="L20" s="41"/>
       <c r="M20" s="41"/>
-      <c r="N20" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M20,Services!$A$1:$B$45,2)),"",VLOOKUP(M20,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O20" s="41"/>
-      <c r="P20" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O20,Services!$A$1:$B$45,2)),"",VLOOKUP(O20,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q20" s="41"/>
-      <c r="R20" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q20,Services!$A$1:$B$45,2)),"",VLOOKUP(Q20,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S20" s="41"/>
-      <c r="T20" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S20,Services!$A$1:$B$45,2)),"",VLOOKUP(S20,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U20" s="41"/>
-      <c r="V20" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U20,Services!$A$1:$B$45,2)),"",VLOOKUP(U20,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W20" s="41"/>
-      <c r="X20" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W20,Services!$A$1:$B$45,2)),"",VLOOKUP(W20,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y20" s="41"/>
-      <c r="Z20" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y20,Services!$A$1:$B$45,2)),"",VLOOKUP(Y20,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA20" s="41"/>
-      <c r="AB20" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA20,Services!$A$1:$B$45,2)),"",VLOOKUP(AA20,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC20" s="41"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="41"/>
+      <c r="Q20" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P20,Services!$A$1:$B$45,2)),"",VLOOKUP(P20,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R20" s="41"/>
+      <c r="S20" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R20,Services!$A$1:$B$45,2)),"",VLOOKUP(R20,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T20" s="41"/>
+      <c r="U20" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T20,Services!$A$1:$B$45,2)),"",VLOOKUP(T20,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V20" s="41"/>
+      <c r="W20" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V20,Services!$A$1:$B$45,2)),"",VLOOKUP(V20,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X20" s="41"/>
+      <c r="Y20" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X20,Services!$A$1:$B$45,2)),"",VLOOKUP(X20,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z20" s="41"/>
+      <c r="AA20" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z20,Services!$A$1:$B$45,2)),"",VLOOKUP(Z20,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB20" s="41"/>
+      <c r="AC20" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB20,Services!$A$1:$B$45,2)),"",VLOOKUP(AB20,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD20" s="41"/>
-    </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE20" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD20,Services!$A$1:$B$45,2)),"",VLOOKUP(AD20,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF20" s="41"/>
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A21" s="41"/>
       <c r="B21" s="41"/>
       <c r="C21" s="42"/>
@@ -9185,49 +9215,51 @@
       <c r="K21" s="41"/>
       <c r="L21" s="41"/>
       <c r="M21" s="41"/>
-      <c r="N21" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M21,Services!$A$1:$B$45,2)),"",VLOOKUP(M21,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O21" s="41"/>
-      <c r="P21" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O21,Services!$A$1:$B$45,2)),"",VLOOKUP(O21,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q21" s="41"/>
-      <c r="R21" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q21,Services!$A$1:$B$45,2)),"",VLOOKUP(Q21,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S21" s="41"/>
-      <c r="T21" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S21,Services!$A$1:$B$45,2)),"",VLOOKUP(S21,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U21" s="41"/>
-      <c r="V21" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U21,Services!$A$1:$B$45,2)),"",VLOOKUP(U21,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W21" s="41"/>
-      <c r="X21" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W21,Services!$A$1:$B$45,2)),"",VLOOKUP(W21,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y21" s="41"/>
-      <c r="Z21" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y21,Services!$A$1:$B$45,2)),"",VLOOKUP(Y21,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA21" s="41"/>
-      <c r="AB21" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA21,Services!$A$1:$B$45,2)),"",VLOOKUP(AA21,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC21" s="41"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="41"/>
+      <c r="Q21" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P21,Services!$A$1:$B$45,2)),"",VLOOKUP(P21,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R21" s="41"/>
+      <c r="S21" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R21,Services!$A$1:$B$45,2)),"",VLOOKUP(R21,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T21" s="41"/>
+      <c r="U21" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T21,Services!$A$1:$B$45,2)),"",VLOOKUP(T21,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V21" s="41"/>
+      <c r="W21" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V21,Services!$A$1:$B$45,2)),"",VLOOKUP(V21,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X21" s="41"/>
+      <c r="Y21" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X21,Services!$A$1:$B$45,2)),"",VLOOKUP(X21,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z21" s="41"/>
+      <c r="AA21" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z21,Services!$A$1:$B$45,2)),"",VLOOKUP(Z21,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB21" s="41"/>
+      <c r="AC21" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB21,Services!$A$1:$B$45,2)),"",VLOOKUP(AB21,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD21" s="41"/>
-    </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE21" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD21,Services!$A$1:$B$45,2)),"",VLOOKUP(AD21,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF21" s="41"/>
+    </row>
+    <row r="22" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A22" s="41"/>
       <c r="B22" s="41"/>
       <c r="C22" s="42"/>
@@ -9250,49 +9282,51 @@
       <c r="K22" s="41"/>
       <c r="L22" s="41"/>
       <c r="M22" s="41"/>
-      <c r="N22" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M22,Services!$A$1:$B$45,2)),"",VLOOKUP(M22,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O22" s="41"/>
-      <c r="P22" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O22,Services!$A$1:$B$45,2)),"",VLOOKUP(O22,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q22" s="41"/>
-      <c r="R22" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q22,Services!$A$1:$B$45,2)),"",VLOOKUP(Q22,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S22" s="41"/>
-      <c r="T22" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S22,Services!$A$1:$B$45,2)),"",VLOOKUP(S22,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U22" s="41"/>
-      <c r="V22" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U22,Services!$A$1:$B$45,2)),"",VLOOKUP(U22,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W22" s="41"/>
-      <c r="X22" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W22,Services!$A$1:$B$45,2)),"",VLOOKUP(W22,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y22" s="41"/>
-      <c r="Z22" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y22,Services!$A$1:$B$45,2)),"",VLOOKUP(Y22,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA22" s="41"/>
-      <c r="AB22" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA22,Services!$A$1:$B$45,2)),"",VLOOKUP(AA22,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC22" s="41"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="41"/>
+      <c r="Q22" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P22,Services!$A$1:$B$45,2)),"",VLOOKUP(P22,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R22" s="41"/>
+      <c r="S22" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R22,Services!$A$1:$B$45,2)),"",VLOOKUP(R22,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T22" s="41"/>
+      <c r="U22" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T22,Services!$A$1:$B$45,2)),"",VLOOKUP(T22,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V22" s="41"/>
+      <c r="W22" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V22,Services!$A$1:$B$45,2)),"",VLOOKUP(V22,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X22" s="41"/>
+      <c r="Y22" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X22,Services!$A$1:$B$45,2)),"",VLOOKUP(X22,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z22" s="41"/>
+      <c r="AA22" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z22,Services!$A$1:$B$45,2)),"",VLOOKUP(Z22,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB22" s="41"/>
+      <c r="AC22" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB22,Services!$A$1:$B$45,2)),"",VLOOKUP(AB22,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD22" s="41"/>
-    </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE22" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD22,Services!$A$1:$B$45,2)),"",VLOOKUP(AD22,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF22" s="41"/>
+    </row>
+    <row r="23" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A23" s="41"/>
       <c r="B23" s="41"/>
       <c r="C23" s="42"/>
@@ -9315,49 +9349,51 @@
       <c r="K23" s="41"/>
       <c r="L23" s="41"/>
       <c r="M23" s="41"/>
-      <c r="N23" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M23,Services!$A$1:$B$45,2)),"",VLOOKUP(M23,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O23" s="41"/>
-      <c r="P23" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O23,Services!$A$1:$B$45,2)),"",VLOOKUP(O23,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q23" s="41"/>
-      <c r="R23" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q23,Services!$A$1:$B$45,2)),"",VLOOKUP(Q23,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S23" s="41"/>
-      <c r="T23" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S23,Services!$A$1:$B$45,2)),"",VLOOKUP(S23,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U23" s="41"/>
-      <c r="V23" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U23,Services!$A$1:$B$45,2)),"",VLOOKUP(U23,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W23" s="41"/>
-      <c r="X23" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W23,Services!$A$1:$B$45,2)),"",VLOOKUP(W23,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y23" s="41"/>
-      <c r="Z23" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y23,Services!$A$1:$B$45,2)),"",VLOOKUP(Y23,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA23" s="41"/>
-      <c r="AB23" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA23,Services!$A$1:$B$45,2)),"",VLOOKUP(AA23,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC23" s="41"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="41"/>
+      <c r="Q23" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P23,Services!$A$1:$B$45,2)),"",VLOOKUP(P23,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R23" s="41"/>
+      <c r="S23" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R23,Services!$A$1:$B$45,2)),"",VLOOKUP(R23,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T23" s="41"/>
+      <c r="U23" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T23,Services!$A$1:$B$45,2)),"",VLOOKUP(T23,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V23" s="41"/>
+      <c r="W23" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V23,Services!$A$1:$B$45,2)),"",VLOOKUP(V23,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X23" s="41"/>
+      <c r="Y23" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X23,Services!$A$1:$B$45,2)),"",VLOOKUP(X23,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z23" s="41"/>
+      <c r="AA23" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z23,Services!$A$1:$B$45,2)),"",VLOOKUP(Z23,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB23" s="41"/>
+      <c r="AC23" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB23,Services!$A$1:$B$45,2)),"",VLOOKUP(AB23,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD23" s="41"/>
-    </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE23" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD23,Services!$A$1:$B$45,2)),"",VLOOKUP(AD23,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF23" s="41"/>
+    </row>
+    <row r="24" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A24" s="41"/>
       <c r="B24" s="41"/>
       <c r="C24" s="42"/>
@@ -9380,49 +9416,51 @@
       <c r="K24" s="41"/>
       <c r="L24" s="41"/>
       <c r="M24" s="41"/>
-      <c r="N24" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M24,Services!$A$1:$B$45,2)),"",VLOOKUP(M24,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O24" s="41"/>
-      <c r="P24" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O24,Services!$A$1:$B$45,2)),"",VLOOKUP(O24,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q24" s="41"/>
-      <c r="R24" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q24,Services!$A$1:$B$45,2)),"",VLOOKUP(Q24,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S24" s="41"/>
-      <c r="T24" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S24,Services!$A$1:$B$45,2)),"",VLOOKUP(S24,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U24" s="41"/>
-      <c r="V24" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U24,Services!$A$1:$B$45,2)),"",VLOOKUP(U24,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W24" s="41"/>
-      <c r="X24" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W24,Services!$A$1:$B$45,2)),"",VLOOKUP(W24,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y24" s="41"/>
-      <c r="Z24" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y24,Services!$A$1:$B$45,2)),"",VLOOKUP(Y24,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA24" s="41"/>
-      <c r="AB24" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA24,Services!$A$1:$B$45,2)),"",VLOOKUP(AA24,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC24" s="41"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="41"/>
+      <c r="Q24" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P24,Services!$A$1:$B$45,2)),"",VLOOKUP(P24,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R24" s="41"/>
+      <c r="S24" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R24,Services!$A$1:$B$45,2)),"",VLOOKUP(R24,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T24" s="41"/>
+      <c r="U24" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T24,Services!$A$1:$B$45,2)),"",VLOOKUP(T24,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V24" s="41"/>
+      <c r="W24" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V24,Services!$A$1:$B$45,2)),"",VLOOKUP(V24,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X24" s="41"/>
+      <c r="Y24" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X24,Services!$A$1:$B$45,2)),"",VLOOKUP(X24,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z24" s="41"/>
+      <c r="AA24" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z24,Services!$A$1:$B$45,2)),"",VLOOKUP(Z24,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB24" s="41"/>
+      <c r="AC24" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB24,Services!$A$1:$B$45,2)),"",VLOOKUP(AB24,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD24" s="41"/>
-    </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE24" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD24,Services!$A$1:$B$45,2)),"",VLOOKUP(AD24,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF24" s="41"/>
+    </row>
+    <row r="25" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A25" s="41"/>
       <c r="B25" s="41"/>
       <c r="C25" s="42"/>
@@ -9445,49 +9483,51 @@
       <c r="K25" s="41"/>
       <c r="L25" s="41"/>
       <c r="M25" s="41"/>
-      <c r="N25" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M25,Services!$A$1:$B$45,2)),"",VLOOKUP(M25,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O25" s="41"/>
-      <c r="P25" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O25,Services!$A$1:$B$45,2)),"",VLOOKUP(O25,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q25" s="41"/>
-      <c r="R25" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q25,Services!$A$1:$B$45,2)),"",VLOOKUP(Q25,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S25" s="41"/>
-      <c r="T25" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S25,Services!$A$1:$B$45,2)),"",VLOOKUP(S25,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U25" s="41"/>
-      <c r="V25" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U25,Services!$A$1:$B$45,2)),"",VLOOKUP(U25,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W25" s="41"/>
-      <c r="X25" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W25,Services!$A$1:$B$45,2)),"",VLOOKUP(W25,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y25" s="41"/>
-      <c r="Z25" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y25,Services!$A$1:$B$45,2)),"",VLOOKUP(Y25,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA25" s="41"/>
-      <c r="AB25" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA25,Services!$A$1:$B$45,2)),"",VLOOKUP(AA25,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC25" s="41"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="41"/>
+      <c r="Q25" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P25,Services!$A$1:$B$45,2)),"",VLOOKUP(P25,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R25" s="41"/>
+      <c r="S25" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R25,Services!$A$1:$B$45,2)),"",VLOOKUP(R25,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T25" s="41"/>
+      <c r="U25" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T25,Services!$A$1:$B$45,2)),"",VLOOKUP(T25,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V25" s="41"/>
+      <c r="W25" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V25,Services!$A$1:$B$45,2)),"",VLOOKUP(V25,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X25" s="41"/>
+      <c r="Y25" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X25,Services!$A$1:$B$45,2)),"",VLOOKUP(X25,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z25" s="41"/>
+      <c r="AA25" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z25,Services!$A$1:$B$45,2)),"",VLOOKUP(Z25,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB25" s="41"/>
+      <c r="AC25" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB25,Services!$A$1:$B$45,2)),"",VLOOKUP(AB25,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD25" s="41"/>
-    </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE25" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD25,Services!$A$1:$B$45,2)),"",VLOOKUP(AD25,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF25" s="41"/>
+    </row>
+    <row r="26" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A26" s="41"/>
       <c r="B26" s="41"/>
       <c r="C26" s="42"/>
@@ -9510,49 +9550,51 @@
       <c r="K26" s="41"/>
       <c r="L26" s="41"/>
       <c r="M26" s="41"/>
-      <c r="N26" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M26,Services!$A$1:$B$45,2)),"",VLOOKUP(M26,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O26" s="41"/>
-      <c r="P26" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O26,Services!$A$1:$B$45,2)),"",VLOOKUP(O26,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q26" s="41"/>
-      <c r="R26" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q26,Services!$A$1:$B$45,2)),"",VLOOKUP(Q26,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S26" s="41"/>
-      <c r="T26" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S26,Services!$A$1:$B$45,2)),"",VLOOKUP(S26,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U26" s="41"/>
-      <c r="V26" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U26,Services!$A$1:$B$45,2)),"",VLOOKUP(U26,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W26" s="41"/>
-      <c r="X26" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W26,Services!$A$1:$B$45,2)),"",VLOOKUP(W26,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y26" s="41"/>
-      <c r="Z26" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y26,Services!$A$1:$B$45,2)),"",VLOOKUP(Y26,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA26" s="41"/>
-      <c r="AB26" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA26,Services!$A$1:$B$45,2)),"",VLOOKUP(AA26,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC26" s="41"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="41"/>
+      <c r="Q26" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P26,Services!$A$1:$B$45,2)),"",VLOOKUP(P26,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R26" s="41"/>
+      <c r="S26" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R26,Services!$A$1:$B$45,2)),"",VLOOKUP(R26,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T26" s="41"/>
+      <c r="U26" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T26,Services!$A$1:$B$45,2)),"",VLOOKUP(T26,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V26" s="41"/>
+      <c r="W26" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V26,Services!$A$1:$B$45,2)),"",VLOOKUP(V26,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X26" s="41"/>
+      <c r="Y26" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X26,Services!$A$1:$B$45,2)),"",VLOOKUP(X26,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z26" s="41"/>
+      <c r="AA26" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z26,Services!$A$1:$B$45,2)),"",VLOOKUP(Z26,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB26" s="41"/>
+      <c r="AC26" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB26,Services!$A$1:$B$45,2)),"",VLOOKUP(AB26,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD26" s="41"/>
-    </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE26" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD26,Services!$A$1:$B$45,2)),"",VLOOKUP(AD26,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF26" s="41"/>
+    </row>
+    <row r="27" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A27" s="41"/>
       <c r="B27" s="41"/>
       <c r="C27" s="42"/>
@@ -9575,49 +9617,51 @@
       <c r="K27" s="41"/>
       <c r="L27" s="41"/>
       <c r="M27" s="41"/>
-      <c r="N27" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M27,Services!$A$1:$B$45,2)),"",VLOOKUP(M27,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O27" s="41"/>
-      <c r="P27" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O27,Services!$A$1:$B$45,2)),"",VLOOKUP(O27,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q27" s="41"/>
-      <c r="R27" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q27,Services!$A$1:$B$45,2)),"",VLOOKUP(Q27,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S27" s="41"/>
-      <c r="T27" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S27,Services!$A$1:$B$45,2)),"",VLOOKUP(S27,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U27" s="41"/>
-      <c r="V27" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U27,Services!$A$1:$B$45,2)),"",VLOOKUP(U27,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W27" s="41"/>
-      <c r="X27" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W27,Services!$A$1:$B$45,2)),"",VLOOKUP(W27,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y27" s="41"/>
-      <c r="Z27" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y27,Services!$A$1:$B$45,2)),"",VLOOKUP(Y27,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA27" s="41"/>
-      <c r="AB27" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA27,Services!$A$1:$B$45,2)),"",VLOOKUP(AA27,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC27" s="41"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="41"/>
+      <c r="Q27" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P27,Services!$A$1:$B$45,2)),"",VLOOKUP(P27,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R27" s="41"/>
+      <c r="S27" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R27,Services!$A$1:$B$45,2)),"",VLOOKUP(R27,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T27" s="41"/>
+      <c r="U27" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T27,Services!$A$1:$B$45,2)),"",VLOOKUP(T27,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V27" s="41"/>
+      <c r="W27" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V27,Services!$A$1:$B$45,2)),"",VLOOKUP(V27,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X27" s="41"/>
+      <c r="Y27" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X27,Services!$A$1:$B$45,2)),"",VLOOKUP(X27,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z27" s="41"/>
+      <c r="AA27" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z27,Services!$A$1:$B$45,2)),"",VLOOKUP(Z27,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB27" s="41"/>
+      <c r="AC27" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB27,Services!$A$1:$B$45,2)),"",VLOOKUP(AB27,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD27" s="41"/>
-    </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE27" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD27,Services!$A$1:$B$45,2)),"",VLOOKUP(AD27,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF27" s="41"/>
+    </row>
+    <row r="28" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A28" s="41"/>
       <c r="B28" s="41"/>
       <c r="C28" s="42"/>
@@ -9640,49 +9684,51 @@
       <c r="K28" s="41"/>
       <c r="L28" s="41"/>
       <c r="M28" s="41"/>
-      <c r="N28" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M28,Services!$A$1:$B$45,2)),"",VLOOKUP(M28,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O28" s="41"/>
-      <c r="P28" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O28,Services!$A$1:$B$45,2)),"",VLOOKUP(O28,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q28" s="41"/>
-      <c r="R28" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q28,Services!$A$1:$B$45,2)),"",VLOOKUP(Q28,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S28" s="41"/>
-      <c r="T28" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S28,Services!$A$1:$B$45,2)),"",VLOOKUP(S28,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U28" s="41"/>
-      <c r="V28" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U28,Services!$A$1:$B$45,2)),"",VLOOKUP(U28,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W28" s="41"/>
-      <c r="X28" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W28,Services!$A$1:$B$45,2)),"",VLOOKUP(W28,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y28" s="41"/>
-      <c r="Z28" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y28,Services!$A$1:$B$45,2)),"",VLOOKUP(Y28,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA28" s="41"/>
-      <c r="AB28" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA28,Services!$A$1:$B$45,2)),"",VLOOKUP(AA28,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC28" s="41"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="41"/>
+      <c r="Q28" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P28,Services!$A$1:$B$45,2)),"",VLOOKUP(P28,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R28" s="41"/>
+      <c r="S28" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R28,Services!$A$1:$B$45,2)),"",VLOOKUP(R28,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T28" s="41"/>
+      <c r="U28" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T28,Services!$A$1:$B$45,2)),"",VLOOKUP(T28,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V28" s="41"/>
+      <c r="W28" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V28,Services!$A$1:$B$45,2)),"",VLOOKUP(V28,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X28" s="41"/>
+      <c r="Y28" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X28,Services!$A$1:$B$45,2)),"",VLOOKUP(X28,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z28" s="41"/>
+      <c r="AA28" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z28,Services!$A$1:$B$45,2)),"",VLOOKUP(Z28,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB28" s="41"/>
+      <c r="AC28" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB28,Services!$A$1:$B$45,2)),"",VLOOKUP(AB28,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD28" s="41"/>
-    </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE28" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD28,Services!$A$1:$B$45,2)),"",VLOOKUP(AD28,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF28" s="41"/>
+    </row>
+    <row r="29" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A29" s="41"/>
       <c r="B29" s="41"/>
       <c r="C29" s="42"/>
@@ -9705,49 +9751,51 @@
       <c r="K29" s="41"/>
       <c r="L29" s="41"/>
       <c r="M29" s="41"/>
-      <c r="N29" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M29,Services!$A$1:$B$45,2)),"",VLOOKUP(M29,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O29" s="41"/>
-      <c r="P29" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O29,Services!$A$1:$B$45,2)),"",VLOOKUP(O29,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q29" s="41"/>
-      <c r="R29" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q29,Services!$A$1:$B$45,2)),"",VLOOKUP(Q29,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S29" s="41"/>
-      <c r="T29" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S29,Services!$A$1:$B$45,2)),"",VLOOKUP(S29,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U29" s="41"/>
-      <c r="V29" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U29,Services!$A$1:$B$45,2)),"",VLOOKUP(U29,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W29" s="41"/>
-      <c r="X29" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W29,Services!$A$1:$B$45,2)),"",VLOOKUP(W29,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y29" s="41"/>
-      <c r="Z29" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y29,Services!$A$1:$B$45,2)),"",VLOOKUP(Y29,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA29" s="41"/>
-      <c r="AB29" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA29,Services!$A$1:$B$45,2)),"",VLOOKUP(AA29,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC29" s="41"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="41"/>
+      <c r="Q29" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P29,Services!$A$1:$B$45,2)),"",VLOOKUP(P29,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R29" s="41"/>
+      <c r="S29" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R29,Services!$A$1:$B$45,2)),"",VLOOKUP(R29,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T29" s="41"/>
+      <c r="U29" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T29,Services!$A$1:$B$45,2)),"",VLOOKUP(T29,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V29" s="41"/>
+      <c r="W29" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V29,Services!$A$1:$B$45,2)),"",VLOOKUP(V29,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X29" s="41"/>
+      <c r="Y29" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X29,Services!$A$1:$B$45,2)),"",VLOOKUP(X29,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z29" s="41"/>
+      <c r="AA29" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z29,Services!$A$1:$B$45,2)),"",VLOOKUP(Z29,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB29" s="41"/>
+      <c r="AC29" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB29,Services!$A$1:$B$45,2)),"",VLOOKUP(AB29,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD29" s="41"/>
-    </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE29" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD29,Services!$A$1:$B$45,2)),"",VLOOKUP(AD29,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF29" s="41"/>
+    </row>
+    <row r="30" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A30" s="41"/>
       <c r="B30" s="41"/>
       <c r="C30" s="42"/>
@@ -9770,49 +9818,51 @@
       <c r="K30" s="41"/>
       <c r="L30" s="41"/>
       <c r="M30" s="41"/>
-      <c r="N30" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M30,Services!$A$1:$B$45,2)),"",VLOOKUP(M30,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O30" s="41"/>
-      <c r="P30" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O30,Services!$A$1:$B$45,2)),"",VLOOKUP(O30,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q30" s="41"/>
-      <c r="R30" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q30,Services!$A$1:$B$45,2)),"",VLOOKUP(Q30,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S30" s="41"/>
-      <c r="T30" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S30,Services!$A$1:$B$45,2)),"",VLOOKUP(S30,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U30" s="41"/>
-      <c r="V30" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U30,Services!$A$1:$B$45,2)),"",VLOOKUP(U30,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W30" s="41"/>
-      <c r="X30" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W30,Services!$A$1:$B$45,2)),"",VLOOKUP(W30,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y30" s="41"/>
-      <c r="Z30" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y30,Services!$A$1:$B$45,2)),"",VLOOKUP(Y30,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA30" s="41"/>
-      <c r="AB30" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA30,Services!$A$1:$B$45,2)),"",VLOOKUP(AA30,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC30" s="41"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="41"/>
+      <c r="Q30" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P30,Services!$A$1:$B$45,2)),"",VLOOKUP(P30,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R30" s="41"/>
+      <c r="S30" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R30,Services!$A$1:$B$45,2)),"",VLOOKUP(R30,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T30" s="41"/>
+      <c r="U30" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T30,Services!$A$1:$B$45,2)),"",VLOOKUP(T30,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V30" s="41"/>
+      <c r="W30" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V30,Services!$A$1:$B$45,2)),"",VLOOKUP(V30,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X30" s="41"/>
+      <c r="Y30" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X30,Services!$A$1:$B$45,2)),"",VLOOKUP(X30,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z30" s="41"/>
+      <c r="AA30" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z30,Services!$A$1:$B$45,2)),"",VLOOKUP(Z30,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB30" s="41"/>
+      <c r="AC30" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB30,Services!$A$1:$B$45,2)),"",VLOOKUP(AB30,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD30" s="41"/>
-    </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE30" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD30,Services!$A$1:$B$45,2)),"",VLOOKUP(AD30,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF30" s="41"/>
+    </row>
+    <row r="31" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A31" s="41"/>
       <c r="B31" s="41"/>
       <c r="C31" s="42"/>
@@ -9835,49 +9885,51 @@
       <c r="K31" s="41"/>
       <c r="L31" s="41"/>
       <c r="M31" s="41"/>
-      <c r="N31" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M31,Services!$A$1:$B$45,2)),"",VLOOKUP(M31,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O31" s="41"/>
-      <c r="P31" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O31,Services!$A$1:$B$45,2)),"",VLOOKUP(O31,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q31" s="41"/>
-      <c r="R31" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q31,Services!$A$1:$B$45,2)),"",VLOOKUP(Q31,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S31" s="41"/>
-      <c r="T31" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S31,Services!$A$1:$B$45,2)),"",VLOOKUP(S31,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U31" s="41"/>
-      <c r="V31" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U31,Services!$A$1:$B$45,2)),"",VLOOKUP(U31,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W31" s="41"/>
-      <c r="X31" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W31,Services!$A$1:$B$45,2)),"",VLOOKUP(W31,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y31" s="41"/>
-      <c r="Z31" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y31,Services!$A$1:$B$45,2)),"",VLOOKUP(Y31,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA31" s="41"/>
-      <c r="AB31" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA31,Services!$A$1:$B$45,2)),"",VLOOKUP(AA31,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC31" s="41"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="41"/>
+      <c r="Q31" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P31,Services!$A$1:$B$45,2)),"",VLOOKUP(P31,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R31" s="41"/>
+      <c r="S31" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R31,Services!$A$1:$B$45,2)),"",VLOOKUP(R31,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T31" s="41"/>
+      <c r="U31" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T31,Services!$A$1:$B$45,2)),"",VLOOKUP(T31,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V31" s="41"/>
+      <c r="W31" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V31,Services!$A$1:$B$45,2)),"",VLOOKUP(V31,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X31" s="41"/>
+      <c r="Y31" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X31,Services!$A$1:$B$45,2)),"",VLOOKUP(X31,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z31" s="41"/>
+      <c r="AA31" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z31,Services!$A$1:$B$45,2)),"",VLOOKUP(Z31,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB31" s="41"/>
+      <c r="AC31" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB31,Services!$A$1:$B$45,2)),"",VLOOKUP(AB31,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD31" s="41"/>
-    </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE31" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD31,Services!$A$1:$B$45,2)),"",VLOOKUP(AD31,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF31" s="41"/>
+    </row>
+    <row r="32" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A32" s="41"/>
       <c r="B32" s="41"/>
       <c r="C32" s="42"/>
@@ -9900,49 +9952,51 @@
       <c r="K32" s="41"/>
       <c r="L32" s="41"/>
       <c r="M32" s="41"/>
-      <c r="N32" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M32,Services!$A$1:$B$45,2)),"",VLOOKUP(M32,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O32" s="41"/>
-      <c r="P32" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O32,Services!$A$1:$B$45,2)),"",VLOOKUP(O32,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q32" s="41"/>
-      <c r="R32" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q32,Services!$A$1:$B$45,2)),"",VLOOKUP(Q32,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S32" s="41"/>
-      <c r="T32" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S32,Services!$A$1:$B$45,2)),"",VLOOKUP(S32,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U32" s="41"/>
-      <c r="V32" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U32,Services!$A$1:$B$45,2)),"",VLOOKUP(U32,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W32" s="41"/>
-      <c r="X32" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W32,Services!$A$1:$B$45,2)),"",VLOOKUP(W32,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y32" s="41"/>
-      <c r="Z32" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y32,Services!$A$1:$B$45,2)),"",VLOOKUP(Y32,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA32" s="41"/>
-      <c r="AB32" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA32,Services!$A$1:$B$45,2)),"",VLOOKUP(AA32,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC32" s="41"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="41"/>
+      <c r="Q32" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P32,Services!$A$1:$B$45,2)),"",VLOOKUP(P32,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R32" s="41"/>
+      <c r="S32" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R32,Services!$A$1:$B$45,2)),"",VLOOKUP(R32,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T32" s="41"/>
+      <c r="U32" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T32,Services!$A$1:$B$45,2)),"",VLOOKUP(T32,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V32" s="41"/>
+      <c r="W32" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V32,Services!$A$1:$B$45,2)),"",VLOOKUP(V32,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X32" s="41"/>
+      <c r="Y32" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X32,Services!$A$1:$B$45,2)),"",VLOOKUP(X32,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z32" s="41"/>
+      <c r="AA32" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z32,Services!$A$1:$B$45,2)),"",VLOOKUP(Z32,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB32" s="41"/>
+      <c r="AC32" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB32,Services!$A$1:$B$45,2)),"",VLOOKUP(AB32,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD32" s="41"/>
-    </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE32" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD32,Services!$A$1:$B$45,2)),"",VLOOKUP(AD32,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF32" s="41"/>
+    </row>
+    <row r="33" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A33" s="41"/>
       <c r="B33" s="41"/>
       <c r="C33" s="42"/>
@@ -9965,49 +10019,51 @@
       <c r="K33" s="41"/>
       <c r="L33" s="41"/>
       <c r="M33" s="41"/>
-      <c r="N33" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M33,Services!$A$1:$B$45,2)),"",VLOOKUP(M33,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O33" s="41"/>
-      <c r="P33" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O33,Services!$A$1:$B$45,2)),"",VLOOKUP(O33,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q33" s="41"/>
-      <c r="R33" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q33,Services!$A$1:$B$45,2)),"",VLOOKUP(Q33,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S33" s="41"/>
-      <c r="T33" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S33,Services!$A$1:$B$45,2)),"",VLOOKUP(S33,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U33" s="41"/>
-      <c r="V33" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U33,Services!$A$1:$B$45,2)),"",VLOOKUP(U33,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W33" s="41"/>
-      <c r="X33" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W33,Services!$A$1:$B$45,2)),"",VLOOKUP(W33,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y33" s="41"/>
-      <c r="Z33" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y33,Services!$A$1:$B$45,2)),"",VLOOKUP(Y33,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA33" s="41"/>
-      <c r="AB33" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA33,Services!$A$1:$B$45,2)),"",VLOOKUP(AA33,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC33" s="41"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="41"/>
+      <c r="Q33" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P33,Services!$A$1:$B$45,2)),"",VLOOKUP(P33,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R33" s="41"/>
+      <c r="S33" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R33,Services!$A$1:$B$45,2)),"",VLOOKUP(R33,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T33" s="41"/>
+      <c r="U33" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T33,Services!$A$1:$B$45,2)),"",VLOOKUP(T33,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V33" s="41"/>
+      <c r="W33" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V33,Services!$A$1:$B$45,2)),"",VLOOKUP(V33,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X33" s="41"/>
+      <c r="Y33" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X33,Services!$A$1:$B$45,2)),"",VLOOKUP(X33,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z33" s="41"/>
+      <c r="AA33" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z33,Services!$A$1:$B$45,2)),"",VLOOKUP(Z33,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB33" s="41"/>
+      <c r="AC33" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB33,Services!$A$1:$B$45,2)),"",VLOOKUP(AB33,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD33" s="41"/>
-    </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE33" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD33,Services!$A$1:$B$45,2)),"",VLOOKUP(AD33,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF33" s="41"/>
+    </row>
+    <row r="34" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A34" s="41"/>
       <c r="B34" s="41"/>
       <c r="C34" s="42"/>
@@ -10030,49 +10086,51 @@
       <c r="K34" s="41"/>
       <c r="L34" s="41"/>
       <c r="M34" s="41"/>
-      <c r="N34" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M34,Services!$A$1:$B$45,2)),"",VLOOKUP(M34,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O34" s="41"/>
-      <c r="P34" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O34,Services!$A$1:$B$45,2)),"",VLOOKUP(O34,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q34" s="41"/>
-      <c r="R34" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q34,Services!$A$1:$B$45,2)),"",VLOOKUP(Q34,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S34" s="41"/>
-      <c r="T34" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S34,Services!$A$1:$B$45,2)),"",VLOOKUP(S34,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U34" s="41"/>
-      <c r="V34" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U34,Services!$A$1:$B$45,2)),"",VLOOKUP(U34,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W34" s="41"/>
-      <c r="X34" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W34,Services!$A$1:$B$45,2)),"",VLOOKUP(W34,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y34" s="41"/>
-      <c r="Z34" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y34,Services!$A$1:$B$45,2)),"",VLOOKUP(Y34,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA34" s="41"/>
-      <c r="AB34" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA34,Services!$A$1:$B$45,2)),"",VLOOKUP(AA34,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC34" s="41"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="41"/>
+      <c r="Q34" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P34,Services!$A$1:$B$45,2)),"",VLOOKUP(P34,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R34" s="41"/>
+      <c r="S34" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R34,Services!$A$1:$B$45,2)),"",VLOOKUP(R34,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T34" s="41"/>
+      <c r="U34" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T34,Services!$A$1:$B$45,2)),"",VLOOKUP(T34,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V34" s="41"/>
+      <c r="W34" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V34,Services!$A$1:$B$45,2)),"",VLOOKUP(V34,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X34" s="41"/>
+      <c r="Y34" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X34,Services!$A$1:$B$45,2)),"",VLOOKUP(X34,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z34" s="41"/>
+      <c r="AA34" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z34,Services!$A$1:$B$45,2)),"",VLOOKUP(Z34,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB34" s="41"/>
+      <c r="AC34" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB34,Services!$A$1:$B$45,2)),"",VLOOKUP(AB34,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD34" s="41"/>
-    </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE34" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD34,Services!$A$1:$B$45,2)),"",VLOOKUP(AD34,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF34" s="41"/>
+    </row>
+    <row r="35" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A35" s="41"/>
       <c r="B35" s="41"/>
       <c r="C35" s="42"/>
@@ -10095,49 +10153,51 @@
       <c r="K35" s="41"/>
       <c r="L35" s="41"/>
       <c r="M35" s="41"/>
-      <c r="N35" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M35,Services!$A$1:$B$45,2)),"",VLOOKUP(M35,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O35" s="41"/>
-      <c r="P35" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O35,Services!$A$1:$B$45,2)),"",VLOOKUP(O35,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q35" s="41"/>
-      <c r="R35" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q35,Services!$A$1:$B$45,2)),"",VLOOKUP(Q35,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S35" s="41"/>
-      <c r="T35" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S35,Services!$A$1:$B$45,2)),"",VLOOKUP(S35,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U35" s="41"/>
-      <c r="V35" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U35,Services!$A$1:$B$45,2)),"",VLOOKUP(U35,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W35" s="41"/>
-      <c r="X35" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W35,Services!$A$1:$B$45,2)),"",VLOOKUP(W35,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y35" s="41"/>
-      <c r="Z35" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y35,Services!$A$1:$B$45,2)),"",VLOOKUP(Y35,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA35" s="41"/>
-      <c r="AB35" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA35,Services!$A$1:$B$45,2)),"",VLOOKUP(AA35,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC35" s="41"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+      <c r="P35" s="41"/>
+      <c r="Q35" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P35,Services!$A$1:$B$45,2)),"",VLOOKUP(P35,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R35" s="41"/>
+      <c r="S35" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R35,Services!$A$1:$B$45,2)),"",VLOOKUP(R35,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T35" s="41"/>
+      <c r="U35" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T35,Services!$A$1:$B$45,2)),"",VLOOKUP(T35,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V35" s="41"/>
+      <c r="W35" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V35,Services!$A$1:$B$45,2)),"",VLOOKUP(V35,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X35" s="41"/>
+      <c r="Y35" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X35,Services!$A$1:$B$45,2)),"",VLOOKUP(X35,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z35" s="41"/>
+      <c r="AA35" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z35,Services!$A$1:$B$45,2)),"",VLOOKUP(Z35,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB35" s="41"/>
+      <c r="AC35" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB35,Services!$A$1:$B$45,2)),"",VLOOKUP(AB35,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD35" s="41"/>
-    </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE35" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD35,Services!$A$1:$B$45,2)),"",VLOOKUP(AD35,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF35" s="41"/>
+    </row>
+    <row r="36" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A36" s="41"/>
       <c r="B36" s="41"/>
       <c r="C36" s="42"/>
@@ -10160,49 +10220,51 @@
       <c r="K36" s="41"/>
       <c r="L36" s="41"/>
       <c r="M36" s="41"/>
-      <c r="N36" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M36,Services!$A$1:$B$45,2)),"",VLOOKUP(M36,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O36" s="41"/>
-      <c r="P36" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O36,Services!$A$1:$B$45,2)),"",VLOOKUP(O36,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q36" s="41"/>
-      <c r="R36" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q36,Services!$A$1:$B$45,2)),"",VLOOKUP(Q36,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S36" s="41"/>
-      <c r="T36" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S36,Services!$A$1:$B$45,2)),"",VLOOKUP(S36,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U36" s="41"/>
-      <c r="V36" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U36,Services!$A$1:$B$45,2)),"",VLOOKUP(U36,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W36" s="41"/>
-      <c r="X36" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W36,Services!$A$1:$B$45,2)),"",VLOOKUP(W36,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y36" s="41"/>
-      <c r="Z36" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y36,Services!$A$1:$B$45,2)),"",VLOOKUP(Y36,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA36" s="41"/>
-      <c r="AB36" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA36,Services!$A$1:$B$45,2)),"",VLOOKUP(AA36,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC36" s="41"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="41"/>
+      <c r="Q36" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P36,Services!$A$1:$B$45,2)),"",VLOOKUP(P36,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R36" s="41"/>
+      <c r="S36" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R36,Services!$A$1:$B$45,2)),"",VLOOKUP(R36,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T36" s="41"/>
+      <c r="U36" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T36,Services!$A$1:$B$45,2)),"",VLOOKUP(T36,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V36" s="41"/>
+      <c r="W36" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V36,Services!$A$1:$B$45,2)),"",VLOOKUP(V36,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X36" s="41"/>
+      <c r="Y36" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X36,Services!$A$1:$B$45,2)),"",VLOOKUP(X36,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z36" s="41"/>
+      <c r="AA36" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z36,Services!$A$1:$B$45,2)),"",VLOOKUP(Z36,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB36" s="41"/>
+      <c r="AC36" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB36,Services!$A$1:$B$45,2)),"",VLOOKUP(AB36,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD36" s="41"/>
-    </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE36" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD36,Services!$A$1:$B$45,2)),"",VLOOKUP(AD36,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF36" s="41"/>
+    </row>
+    <row r="37" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A37" s="41"/>
       <c r="B37" s="41"/>
       <c r="C37" s="42"/>
@@ -10225,49 +10287,51 @@
       <c r="K37" s="41"/>
       <c r="L37" s="41"/>
       <c r="M37" s="41"/>
-      <c r="N37" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M37,Services!$A$1:$B$45,2)),"",VLOOKUP(M37,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O37" s="41"/>
-      <c r="P37" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O37,Services!$A$1:$B$45,2)),"",VLOOKUP(O37,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q37" s="41"/>
-      <c r="R37" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q37,Services!$A$1:$B$45,2)),"",VLOOKUP(Q37,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S37" s="41"/>
-      <c r="T37" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S37,Services!$A$1:$B$45,2)),"",VLOOKUP(S37,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U37" s="41"/>
-      <c r="V37" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U37,Services!$A$1:$B$45,2)),"",VLOOKUP(U37,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W37" s="41"/>
-      <c r="X37" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W37,Services!$A$1:$B$45,2)),"",VLOOKUP(W37,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y37" s="41"/>
-      <c r="Z37" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y37,Services!$A$1:$B$45,2)),"",VLOOKUP(Y37,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA37" s="41"/>
-      <c r="AB37" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA37,Services!$A$1:$B$45,2)),"",VLOOKUP(AA37,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC37" s="41"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="41"/>
+      <c r="Q37" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P37,Services!$A$1:$B$45,2)),"",VLOOKUP(P37,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R37" s="41"/>
+      <c r="S37" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R37,Services!$A$1:$B$45,2)),"",VLOOKUP(R37,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T37" s="41"/>
+      <c r="U37" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T37,Services!$A$1:$B$45,2)),"",VLOOKUP(T37,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V37" s="41"/>
+      <c r="W37" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V37,Services!$A$1:$B$45,2)),"",VLOOKUP(V37,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X37" s="41"/>
+      <c r="Y37" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X37,Services!$A$1:$B$45,2)),"",VLOOKUP(X37,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z37" s="41"/>
+      <c r="AA37" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z37,Services!$A$1:$B$45,2)),"",VLOOKUP(Z37,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB37" s="41"/>
+      <c r="AC37" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB37,Services!$A$1:$B$45,2)),"",VLOOKUP(AB37,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD37" s="41"/>
-    </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE37" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD37,Services!$A$1:$B$45,2)),"",VLOOKUP(AD37,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF37" s="41"/>
+    </row>
+    <row r="38" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A38" s="41"/>
       <c r="B38" s="41"/>
       <c r="C38" s="42"/>
@@ -10290,49 +10354,51 @@
       <c r="K38" s="41"/>
       <c r="L38" s="41"/>
       <c r="M38" s="41"/>
-      <c r="N38" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M38,Services!$A$1:$B$45,2)),"",VLOOKUP(M38,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O38" s="41"/>
-      <c r="P38" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O38,Services!$A$1:$B$45,2)),"",VLOOKUP(O38,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q38" s="41"/>
-      <c r="R38" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q38,Services!$A$1:$B$45,2)),"",VLOOKUP(Q38,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S38" s="41"/>
-      <c r="T38" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S38,Services!$A$1:$B$45,2)),"",VLOOKUP(S38,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U38" s="41"/>
-      <c r="V38" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U38,Services!$A$1:$B$45,2)),"",VLOOKUP(U38,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W38" s="41"/>
-      <c r="X38" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W38,Services!$A$1:$B$45,2)),"",VLOOKUP(W38,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y38" s="41"/>
-      <c r="Z38" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y38,Services!$A$1:$B$45,2)),"",VLOOKUP(Y38,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA38" s="41"/>
-      <c r="AB38" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA38,Services!$A$1:$B$45,2)),"",VLOOKUP(AA38,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC38" s="41"/>
+      <c r="N38" s="1"/>
+      <c r="O38" s="1"/>
+      <c r="P38" s="41"/>
+      <c r="Q38" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P38,Services!$A$1:$B$45,2)),"",VLOOKUP(P38,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R38" s="41"/>
+      <c r="S38" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R38,Services!$A$1:$B$45,2)),"",VLOOKUP(R38,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T38" s="41"/>
+      <c r="U38" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T38,Services!$A$1:$B$45,2)),"",VLOOKUP(T38,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V38" s="41"/>
+      <c r="W38" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V38,Services!$A$1:$B$45,2)),"",VLOOKUP(V38,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X38" s="41"/>
+      <c r="Y38" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X38,Services!$A$1:$B$45,2)),"",VLOOKUP(X38,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z38" s="41"/>
+      <c r="AA38" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z38,Services!$A$1:$B$45,2)),"",VLOOKUP(Z38,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB38" s="41"/>
+      <c r="AC38" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB38,Services!$A$1:$B$45,2)),"",VLOOKUP(AB38,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD38" s="41"/>
-    </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE38" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD38,Services!$A$1:$B$45,2)),"",VLOOKUP(AD38,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF38" s="41"/>
+    </row>
+    <row r="39" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A39" s="41"/>
       <c r="B39" s="41"/>
       <c r="C39" s="42"/>
@@ -10355,49 +10421,51 @@
       <c r="K39" s="41"/>
       <c r="L39" s="41"/>
       <c r="M39" s="41"/>
-      <c r="N39" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M39,Services!$A$1:$B$45,2)),"",VLOOKUP(M39,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O39" s="41"/>
-      <c r="P39" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O39,Services!$A$1:$B$45,2)),"",VLOOKUP(O39,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q39" s="41"/>
-      <c r="R39" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q39,Services!$A$1:$B$45,2)),"",VLOOKUP(Q39,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S39" s="41"/>
-      <c r="T39" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S39,Services!$A$1:$B$45,2)),"",VLOOKUP(S39,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U39" s="41"/>
-      <c r="V39" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U39,Services!$A$1:$B$45,2)),"",VLOOKUP(U39,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W39" s="41"/>
-      <c r="X39" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W39,Services!$A$1:$B$45,2)),"",VLOOKUP(W39,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y39" s="41"/>
-      <c r="Z39" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y39,Services!$A$1:$B$45,2)),"",VLOOKUP(Y39,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA39" s="41"/>
-      <c r="AB39" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA39,Services!$A$1:$B$45,2)),"",VLOOKUP(AA39,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC39" s="41"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="1"/>
+      <c r="P39" s="41"/>
+      <c r="Q39" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P39,Services!$A$1:$B$45,2)),"",VLOOKUP(P39,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R39" s="41"/>
+      <c r="S39" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R39,Services!$A$1:$B$45,2)),"",VLOOKUP(R39,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T39" s="41"/>
+      <c r="U39" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T39,Services!$A$1:$B$45,2)),"",VLOOKUP(T39,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V39" s="41"/>
+      <c r="W39" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V39,Services!$A$1:$B$45,2)),"",VLOOKUP(V39,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X39" s="41"/>
+      <c r="Y39" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X39,Services!$A$1:$B$45,2)),"",VLOOKUP(X39,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z39" s="41"/>
+      <c r="AA39" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z39,Services!$A$1:$B$45,2)),"",VLOOKUP(Z39,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB39" s="41"/>
+      <c r="AC39" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB39,Services!$A$1:$B$45,2)),"",VLOOKUP(AB39,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD39" s="41"/>
-    </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE39" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD39,Services!$A$1:$B$45,2)),"",VLOOKUP(AD39,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF39" s="41"/>
+    </row>
+    <row r="40" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A40" s="41"/>
       <c r="B40" s="41"/>
       <c r="C40" s="42"/>
@@ -10420,49 +10488,51 @@
       <c r="K40" s="41"/>
       <c r="L40" s="41"/>
       <c r="M40" s="41"/>
-      <c r="N40" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M40,Services!$A$1:$B$45,2)),"",VLOOKUP(M40,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O40" s="41"/>
-      <c r="P40" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O40,Services!$A$1:$B$45,2)),"",VLOOKUP(O40,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q40" s="41"/>
-      <c r="R40" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q40,Services!$A$1:$B$45,2)),"",VLOOKUP(Q40,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S40" s="41"/>
-      <c r="T40" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S40,Services!$A$1:$B$45,2)),"",VLOOKUP(S40,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U40" s="41"/>
-      <c r="V40" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U40,Services!$A$1:$B$45,2)),"",VLOOKUP(U40,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W40" s="41"/>
-      <c r="X40" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W40,Services!$A$1:$B$45,2)),"",VLOOKUP(W40,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y40" s="41"/>
-      <c r="Z40" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y40,Services!$A$1:$B$45,2)),"",VLOOKUP(Y40,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA40" s="41"/>
-      <c r="AB40" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA40,Services!$A$1:$B$45,2)),"",VLOOKUP(AA40,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC40" s="41"/>
+      <c r="N40" s="1"/>
+      <c r="O40" s="1"/>
+      <c r="P40" s="41"/>
+      <c r="Q40" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P40,Services!$A$1:$B$45,2)),"",VLOOKUP(P40,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R40" s="41"/>
+      <c r="S40" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R40,Services!$A$1:$B$45,2)),"",VLOOKUP(R40,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T40" s="41"/>
+      <c r="U40" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T40,Services!$A$1:$B$45,2)),"",VLOOKUP(T40,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V40" s="41"/>
+      <c r="W40" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V40,Services!$A$1:$B$45,2)),"",VLOOKUP(V40,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X40" s="41"/>
+      <c r="Y40" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X40,Services!$A$1:$B$45,2)),"",VLOOKUP(X40,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z40" s="41"/>
+      <c r="AA40" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z40,Services!$A$1:$B$45,2)),"",VLOOKUP(Z40,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB40" s="41"/>
+      <c r="AC40" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB40,Services!$A$1:$B$45,2)),"",VLOOKUP(AB40,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD40" s="41"/>
-    </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE40" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD40,Services!$A$1:$B$45,2)),"",VLOOKUP(AD40,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF40" s="41"/>
+    </row>
+    <row r="41" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A41" s="41"/>
       <c r="B41" s="41"/>
       <c r="C41" s="42"/>
@@ -10485,49 +10555,51 @@
       <c r="K41" s="41"/>
       <c r="L41" s="41"/>
       <c r="M41" s="41"/>
-      <c r="N41" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M41,Services!$A$1:$B$45,2)),"",VLOOKUP(M41,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O41" s="41"/>
-      <c r="P41" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O41,Services!$A$1:$B$45,2)),"",VLOOKUP(O41,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q41" s="41"/>
-      <c r="R41" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q41,Services!$A$1:$B$45,2)),"",VLOOKUP(Q41,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S41" s="41"/>
-      <c r="T41" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S41,Services!$A$1:$B$45,2)),"",VLOOKUP(S41,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U41" s="41"/>
-      <c r="V41" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U41,Services!$A$1:$B$45,2)),"",VLOOKUP(U41,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W41" s="41"/>
-      <c r="X41" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W41,Services!$A$1:$B$45,2)),"",VLOOKUP(W41,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y41" s="41"/>
-      <c r="Z41" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y41,Services!$A$1:$B$45,2)),"",VLOOKUP(Y41,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA41" s="41"/>
-      <c r="AB41" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA41,Services!$A$1:$B$45,2)),"",VLOOKUP(AA41,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC41" s="41"/>
+      <c r="N41" s="1"/>
+      <c r="O41" s="1"/>
+      <c r="P41" s="41"/>
+      <c r="Q41" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P41,Services!$A$1:$B$45,2)),"",VLOOKUP(P41,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R41" s="41"/>
+      <c r="S41" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R41,Services!$A$1:$B$45,2)),"",VLOOKUP(R41,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T41" s="41"/>
+      <c r="U41" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T41,Services!$A$1:$B$45,2)),"",VLOOKUP(T41,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V41" s="41"/>
+      <c r="W41" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V41,Services!$A$1:$B$45,2)),"",VLOOKUP(V41,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X41" s="41"/>
+      <c r="Y41" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X41,Services!$A$1:$B$45,2)),"",VLOOKUP(X41,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z41" s="41"/>
+      <c r="AA41" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z41,Services!$A$1:$B$45,2)),"",VLOOKUP(Z41,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB41" s="41"/>
+      <c r="AC41" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB41,Services!$A$1:$B$45,2)),"",VLOOKUP(AB41,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD41" s="41"/>
-    </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE41" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD41,Services!$A$1:$B$45,2)),"",VLOOKUP(AD41,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF41" s="41"/>
+    </row>
+    <row r="42" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A42" s="41"/>
       <c r="B42" s="41"/>
       <c r="C42" s="42"/>
@@ -10550,49 +10622,51 @@
       <c r="K42" s="41"/>
       <c r="L42" s="41"/>
       <c r="M42" s="41"/>
-      <c r="N42" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M42,Services!$A$1:$B$45,2)),"",VLOOKUP(M42,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O42" s="41"/>
-      <c r="P42" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O42,Services!$A$1:$B$45,2)),"",VLOOKUP(O42,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q42" s="41"/>
-      <c r="R42" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q42,Services!$A$1:$B$45,2)),"",VLOOKUP(Q42,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S42" s="41"/>
-      <c r="T42" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S42,Services!$A$1:$B$45,2)),"",VLOOKUP(S42,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U42" s="41"/>
-      <c r="V42" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U42,Services!$A$1:$B$45,2)),"",VLOOKUP(U42,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W42" s="41"/>
-      <c r="X42" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W42,Services!$A$1:$B$45,2)),"",VLOOKUP(W42,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y42" s="41"/>
-      <c r="Z42" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y42,Services!$A$1:$B$45,2)),"",VLOOKUP(Y42,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA42" s="41"/>
-      <c r="AB42" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA42,Services!$A$1:$B$45,2)),"",VLOOKUP(AA42,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC42" s="41"/>
+      <c r="N42" s="1"/>
+      <c r="O42" s="1"/>
+      <c r="P42" s="41"/>
+      <c r="Q42" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P42,Services!$A$1:$B$45,2)),"",VLOOKUP(P42,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R42" s="41"/>
+      <c r="S42" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R42,Services!$A$1:$B$45,2)),"",VLOOKUP(R42,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T42" s="41"/>
+      <c r="U42" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T42,Services!$A$1:$B$45,2)),"",VLOOKUP(T42,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V42" s="41"/>
+      <c r="W42" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V42,Services!$A$1:$B$45,2)),"",VLOOKUP(V42,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X42" s="41"/>
+      <c r="Y42" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X42,Services!$A$1:$B$45,2)),"",VLOOKUP(X42,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z42" s="41"/>
+      <c r="AA42" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z42,Services!$A$1:$B$45,2)),"",VLOOKUP(Z42,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB42" s="41"/>
+      <c r="AC42" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB42,Services!$A$1:$B$45,2)),"",VLOOKUP(AB42,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD42" s="41"/>
-    </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE42" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD42,Services!$A$1:$B$45,2)),"",VLOOKUP(AD42,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF42" s="41"/>
+    </row>
+    <row r="43" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A43" s="41"/>
       <c r="B43" s="41"/>
       <c r="C43" s="42"/>
@@ -10615,49 +10689,51 @@
       <c r="K43" s="41"/>
       <c r="L43" s="41"/>
       <c r="M43" s="41"/>
-      <c r="N43" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M43,Services!$A$1:$B$45,2)),"",VLOOKUP(M43,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O43" s="41"/>
-      <c r="P43" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O43,Services!$A$1:$B$45,2)),"",VLOOKUP(O43,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q43" s="41"/>
-      <c r="R43" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q43,Services!$A$1:$B$45,2)),"",VLOOKUP(Q43,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S43" s="41"/>
-      <c r="T43" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S43,Services!$A$1:$B$45,2)),"",VLOOKUP(S43,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U43" s="41"/>
-      <c r="V43" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U43,Services!$A$1:$B$45,2)),"",VLOOKUP(U43,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W43" s="41"/>
-      <c r="X43" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W43,Services!$A$1:$B$45,2)),"",VLOOKUP(W43,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y43" s="41"/>
-      <c r="Z43" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y43,Services!$A$1:$B$45,2)),"",VLOOKUP(Y43,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA43" s="41"/>
-      <c r="AB43" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA43,Services!$A$1:$B$45,2)),"",VLOOKUP(AA43,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC43" s="41"/>
+      <c r="N43" s="1"/>
+      <c r="O43" s="1"/>
+      <c r="P43" s="41"/>
+      <c r="Q43" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P43,Services!$A$1:$B$45,2)),"",VLOOKUP(P43,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R43" s="41"/>
+      <c r="S43" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R43,Services!$A$1:$B$45,2)),"",VLOOKUP(R43,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T43" s="41"/>
+      <c r="U43" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T43,Services!$A$1:$B$45,2)),"",VLOOKUP(T43,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V43" s="41"/>
+      <c r="W43" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V43,Services!$A$1:$B$45,2)),"",VLOOKUP(V43,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X43" s="41"/>
+      <c r="Y43" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X43,Services!$A$1:$B$45,2)),"",VLOOKUP(X43,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z43" s="41"/>
+      <c r="AA43" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z43,Services!$A$1:$B$45,2)),"",VLOOKUP(Z43,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB43" s="41"/>
+      <c r="AC43" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB43,Services!$A$1:$B$45,2)),"",VLOOKUP(AB43,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD43" s="41"/>
-    </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE43" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD43,Services!$A$1:$B$45,2)),"",VLOOKUP(AD43,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF43" s="41"/>
+    </row>
+    <row r="44" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A44" s="41"/>
       <c r="B44" s="41"/>
       <c r="C44" s="42"/>
@@ -10680,49 +10756,51 @@
       <c r="K44" s="41"/>
       <c r="L44" s="41"/>
       <c r="M44" s="41"/>
-      <c r="N44" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M44,Services!$A$1:$B$45,2)),"",VLOOKUP(M44,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O44" s="41"/>
-      <c r="P44" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O44,Services!$A$1:$B$45,2)),"",VLOOKUP(O44,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q44" s="41"/>
-      <c r="R44" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q44,Services!$A$1:$B$45,2)),"",VLOOKUP(Q44,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S44" s="41"/>
-      <c r="T44" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S44,Services!$A$1:$B$45,2)),"",VLOOKUP(S44,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U44" s="41"/>
-      <c r="V44" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U44,Services!$A$1:$B$45,2)),"",VLOOKUP(U44,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W44" s="41"/>
-      <c r="X44" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W44,Services!$A$1:$B$45,2)),"",VLOOKUP(W44,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y44" s="41"/>
-      <c r="Z44" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y44,Services!$A$1:$B$45,2)),"",VLOOKUP(Y44,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA44" s="41"/>
-      <c r="AB44" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA44,Services!$A$1:$B$45,2)),"",VLOOKUP(AA44,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC44" s="41"/>
+      <c r="N44" s="1"/>
+      <c r="O44" s="1"/>
+      <c r="P44" s="41"/>
+      <c r="Q44" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P44,Services!$A$1:$B$45,2)),"",VLOOKUP(P44,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R44" s="41"/>
+      <c r="S44" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R44,Services!$A$1:$B$45,2)),"",VLOOKUP(R44,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T44" s="41"/>
+      <c r="U44" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T44,Services!$A$1:$B$45,2)),"",VLOOKUP(T44,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V44" s="41"/>
+      <c r="W44" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V44,Services!$A$1:$B$45,2)),"",VLOOKUP(V44,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X44" s="41"/>
+      <c r="Y44" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X44,Services!$A$1:$B$45,2)),"",VLOOKUP(X44,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z44" s="41"/>
+      <c r="AA44" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z44,Services!$A$1:$B$45,2)),"",VLOOKUP(Z44,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB44" s="41"/>
+      <c r="AC44" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB44,Services!$A$1:$B$45,2)),"",VLOOKUP(AB44,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD44" s="41"/>
-    </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE44" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD44,Services!$A$1:$B$45,2)),"",VLOOKUP(AD44,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF44" s="41"/>
+    </row>
+    <row r="45" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A45" s="41"/>
       <c r="B45" s="41"/>
       <c r="C45" s="42"/>
@@ -10745,49 +10823,51 @@
       <c r="K45" s="41"/>
       <c r="L45" s="41"/>
       <c r="M45" s="41"/>
-      <c r="N45" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M45,Services!$A$1:$B$45,2)),"",VLOOKUP(M45,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O45" s="41"/>
-      <c r="P45" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O45,Services!$A$1:$B$45,2)),"",VLOOKUP(O45,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q45" s="41"/>
-      <c r="R45" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q45,Services!$A$1:$B$45,2)),"",VLOOKUP(Q45,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S45" s="41"/>
-      <c r="T45" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S45,Services!$A$1:$B$45,2)),"",VLOOKUP(S45,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U45" s="41"/>
-      <c r="V45" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U45,Services!$A$1:$B$45,2)),"",VLOOKUP(U45,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W45" s="41"/>
-      <c r="X45" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W45,Services!$A$1:$B$45,2)),"",VLOOKUP(W45,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y45" s="41"/>
-      <c r="Z45" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y45,Services!$A$1:$B$45,2)),"",VLOOKUP(Y45,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA45" s="41"/>
-      <c r="AB45" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA45,Services!$A$1:$B$45,2)),"",VLOOKUP(AA45,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC45" s="41"/>
+      <c r="N45" s="1"/>
+      <c r="O45" s="1"/>
+      <c r="P45" s="41"/>
+      <c r="Q45" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P45,Services!$A$1:$B$45,2)),"",VLOOKUP(P45,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R45" s="41"/>
+      <c r="S45" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R45,Services!$A$1:$B$45,2)),"",VLOOKUP(R45,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T45" s="41"/>
+      <c r="U45" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T45,Services!$A$1:$B$45,2)),"",VLOOKUP(T45,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V45" s="41"/>
+      <c r="W45" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V45,Services!$A$1:$B$45,2)),"",VLOOKUP(V45,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X45" s="41"/>
+      <c r="Y45" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X45,Services!$A$1:$B$45,2)),"",VLOOKUP(X45,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z45" s="41"/>
+      <c r="AA45" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z45,Services!$A$1:$B$45,2)),"",VLOOKUP(Z45,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB45" s="41"/>
+      <c r="AC45" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB45,Services!$A$1:$B$45,2)),"",VLOOKUP(AB45,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD45" s="41"/>
-    </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE45" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD45,Services!$A$1:$B$45,2)),"",VLOOKUP(AD45,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF45" s="41"/>
+    </row>
+    <row r="46" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A46" s="41"/>
       <c r="B46" s="41"/>
       <c r="C46" s="42"/>
@@ -10810,49 +10890,51 @@
       <c r="K46" s="41"/>
       <c r="L46" s="41"/>
       <c r="M46" s="41"/>
-      <c r="N46" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M46,Services!$A$1:$B$45,2)),"",VLOOKUP(M46,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O46" s="41"/>
-      <c r="P46" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O46,Services!$A$1:$B$45,2)),"",VLOOKUP(O46,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q46" s="41"/>
-      <c r="R46" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q46,Services!$A$1:$B$45,2)),"",VLOOKUP(Q46,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S46" s="41"/>
-      <c r="T46" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S46,Services!$A$1:$B$45,2)),"",VLOOKUP(S46,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U46" s="41"/>
-      <c r="V46" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U46,Services!$A$1:$B$45,2)),"",VLOOKUP(U46,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W46" s="41"/>
-      <c r="X46" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W46,Services!$A$1:$B$45,2)),"",VLOOKUP(W46,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y46" s="41"/>
-      <c r="Z46" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y46,Services!$A$1:$B$45,2)),"",VLOOKUP(Y46,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA46" s="41"/>
-      <c r="AB46" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA46,Services!$A$1:$B$45,2)),"",VLOOKUP(AA46,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC46" s="41"/>
+      <c r="N46" s="1"/>
+      <c r="O46" s="1"/>
+      <c r="P46" s="41"/>
+      <c r="Q46" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P46,Services!$A$1:$B$45,2)),"",VLOOKUP(P46,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R46" s="41"/>
+      <c r="S46" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R46,Services!$A$1:$B$45,2)),"",VLOOKUP(R46,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T46" s="41"/>
+      <c r="U46" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T46,Services!$A$1:$B$45,2)),"",VLOOKUP(T46,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V46" s="41"/>
+      <c r="W46" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V46,Services!$A$1:$B$45,2)),"",VLOOKUP(V46,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X46" s="41"/>
+      <c r="Y46" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X46,Services!$A$1:$B$45,2)),"",VLOOKUP(X46,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z46" s="41"/>
+      <c r="AA46" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z46,Services!$A$1:$B$45,2)),"",VLOOKUP(Z46,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB46" s="41"/>
+      <c r="AC46" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB46,Services!$A$1:$B$45,2)),"",VLOOKUP(AB46,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD46" s="41"/>
-    </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE46" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD46,Services!$A$1:$B$45,2)),"",VLOOKUP(AD46,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF46" s="41"/>
+    </row>
+    <row r="47" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A47" s="41"/>
       <c r="B47" s="41"/>
       <c r="C47" s="42"/>
@@ -10875,49 +10957,51 @@
       <c r="K47" s="41"/>
       <c r="L47" s="41"/>
       <c r="M47" s="41"/>
-      <c r="N47" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M47,Services!$A$1:$B$45,2)),"",VLOOKUP(M47,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O47" s="41"/>
-      <c r="P47" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O47,Services!$A$1:$B$45,2)),"",VLOOKUP(O47,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q47" s="41"/>
-      <c r="R47" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q47,Services!$A$1:$B$45,2)),"",VLOOKUP(Q47,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S47" s="41"/>
-      <c r="T47" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S47,Services!$A$1:$B$45,2)),"",VLOOKUP(S47,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U47" s="41"/>
-      <c r="V47" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U47,Services!$A$1:$B$45,2)),"",VLOOKUP(U47,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W47" s="41"/>
-      <c r="X47" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W47,Services!$A$1:$B$45,2)),"",VLOOKUP(W47,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y47" s="41"/>
-      <c r="Z47" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y47,Services!$A$1:$B$45,2)),"",VLOOKUP(Y47,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA47" s="41"/>
-      <c r="AB47" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA47,Services!$A$1:$B$45,2)),"",VLOOKUP(AA47,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC47" s="41"/>
+      <c r="N47" s="1"/>
+      <c r="O47" s="1"/>
+      <c r="P47" s="41"/>
+      <c r="Q47" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P47,Services!$A$1:$B$45,2)),"",VLOOKUP(P47,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R47" s="41"/>
+      <c r="S47" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R47,Services!$A$1:$B$45,2)),"",VLOOKUP(R47,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T47" s="41"/>
+      <c r="U47" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T47,Services!$A$1:$B$45,2)),"",VLOOKUP(T47,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V47" s="41"/>
+      <c r="W47" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V47,Services!$A$1:$B$45,2)),"",VLOOKUP(V47,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X47" s="41"/>
+      <c r="Y47" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X47,Services!$A$1:$B$45,2)),"",VLOOKUP(X47,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z47" s="41"/>
+      <c r="AA47" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z47,Services!$A$1:$B$45,2)),"",VLOOKUP(Z47,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB47" s="41"/>
+      <c r="AC47" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB47,Services!$A$1:$B$45,2)),"",VLOOKUP(AB47,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD47" s="41"/>
-    </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE47" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD47,Services!$A$1:$B$45,2)),"",VLOOKUP(AD47,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF47" s="41"/>
+    </row>
+    <row r="48" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A48" s="41"/>
       <c r="B48" s="41"/>
       <c r="C48" s="42"/>
@@ -10940,49 +11024,51 @@
       <c r="K48" s="41"/>
       <c r="L48" s="41"/>
       <c r="M48" s="41"/>
-      <c r="N48" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M48,Services!$A$1:$B$45,2)),"",VLOOKUP(M48,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O48" s="41"/>
-      <c r="P48" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O48,Services!$A$1:$B$45,2)),"",VLOOKUP(O48,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q48" s="41"/>
-      <c r="R48" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q48,Services!$A$1:$B$45,2)),"",VLOOKUP(Q48,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S48" s="41"/>
-      <c r="T48" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S48,Services!$A$1:$B$45,2)),"",VLOOKUP(S48,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U48" s="41"/>
-      <c r="V48" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U48,Services!$A$1:$B$45,2)),"",VLOOKUP(U48,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W48" s="41"/>
-      <c r="X48" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W48,Services!$A$1:$B$45,2)),"",VLOOKUP(W48,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y48" s="41"/>
-      <c r="Z48" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y48,Services!$A$1:$B$45,2)),"",VLOOKUP(Y48,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA48" s="41"/>
-      <c r="AB48" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA48,Services!$A$1:$B$45,2)),"",VLOOKUP(AA48,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC48" s="41"/>
+      <c r="N48" s="1"/>
+      <c r="O48" s="1"/>
+      <c r="P48" s="41"/>
+      <c r="Q48" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P48,Services!$A$1:$B$45,2)),"",VLOOKUP(P48,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R48" s="41"/>
+      <c r="S48" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R48,Services!$A$1:$B$45,2)),"",VLOOKUP(R48,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T48" s="41"/>
+      <c r="U48" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T48,Services!$A$1:$B$45,2)),"",VLOOKUP(T48,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V48" s="41"/>
+      <c r="W48" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V48,Services!$A$1:$B$45,2)),"",VLOOKUP(V48,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X48" s="41"/>
+      <c r="Y48" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X48,Services!$A$1:$B$45,2)),"",VLOOKUP(X48,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z48" s="41"/>
+      <c r="AA48" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z48,Services!$A$1:$B$45,2)),"",VLOOKUP(Z48,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB48" s="41"/>
+      <c r="AC48" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB48,Services!$A$1:$B$45,2)),"",VLOOKUP(AB48,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD48" s="41"/>
-    </row>
-    <row r="49" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE48" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD48,Services!$A$1:$B$45,2)),"",VLOOKUP(AD48,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF48" s="41"/>
+    </row>
+    <row r="49" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A49" s="41"/>
       <c r="B49" s="41"/>
       <c r="C49" s="42"/>
@@ -11005,49 +11091,51 @@
       <c r="K49" s="41"/>
       <c r="L49" s="41"/>
       <c r="M49" s="41"/>
-      <c r="N49" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M49,Services!$A$1:$B$45,2)),"",VLOOKUP(M49,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O49" s="41"/>
-      <c r="P49" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O49,Services!$A$1:$B$45,2)),"",VLOOKUP(O49,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q49" s="41"/>
-      <c r="R49" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q49,Services!$A$1:$B$45,2)),"",VLOOKUP(Q49,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S49" s="41"/>
-      <c r="T49" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S49,Services!$A$1:$B$45,2)),"",VLOOKUP(S49,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U49" s="41"/>
-      <c r="V49" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U49,Services!$A$1:$B$45,2)),"",VLOOKUP(U49,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W49" s="41"/>
-      <c r="X49" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W49,Services!$A$1:$B$45,2)),"",VLOOKUP(W49,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y49" s="41"/>
-      <c r="Z49" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y49,Services!$A$1:$B$45,2)),"",VLOOKUP(Y49,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA49" s="41"/>
-      <c r="AB49" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA49,Services!$A$1:$B$45,2)),"",VLOOKUP(AA49,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC49" s="41"/>
+      <c r="N49" s="1"/>
+      <c r="O49" s="1"/>
+      <c r="P49" s="41"/>
+      <c r="Q49" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P49,Services!$A$1:$B$45,2)),"",VLOOKUP(P49,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R49" s="41"/>
+      <c r="S49" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R49,Services!$A$1:$B$45,2)),"",VLOOKUP(R49,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T49" s="41"/>
+      <c r="U49" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T49,Services!$A$1:$B$45,2)),"",VLOOKUP(T49,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V49" s="41"/>
+      <c r="W49" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V49,Services!$A$1:$B$45,2)),"",VLOOKUP(V49,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X49" s="41"/>
+      <c r="Y49" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X49,Services!$A$1:$B$45,2)),"",VLOOKUP(X49,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z49" s="41"/>
+      <c r="AA49" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z49,Services!$A$1:$B$45,2)),"",VLOOKUP(Z49,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB49" s="41"/>
+      <c r="AC49" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB49,Services!$A$1:$B$45,2)),"",VLOOKUP(AB49,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD49" s="41"/>
-    </row>
-    <row r="50" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE49" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD49,Services!$A$1:$B$45,2)),"",VLOOKUP(AD49,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF49" s="41"/>
+    </row>
+    <row r="50" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A50" s="41"/>
       <c r="B50" s="41"/>
       <c r="C50" s="42"/>
@@ -11070,47 +11158,49 @@
       <c r="K50" s="41"/>
       <c r="L50" s="41"/>
       <c r="M50" s="41"/>
-      <c r="N50" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M50,Services!$A$1:$B$45,2)),"",VLOOKUP(M50,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O50" s="41"/>
-      <c r="P50" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O50,Services!$A$1:$B$45,2)),"",VLOOKUP(O50,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q50" s="41"/>
-      <c r="R50" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q50,Services!$A$1:$B$45,2)),"",VLOOKUP(Q50,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S50" s="41"/>
-      <c r="T50" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S50,Services!$A$1:$B$45,2)),"",VLOOKUP(S50,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U50" s="41"/>
-      <c r="V50" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U50,Services!$A$1:$B$45,2)),"",VLOOKUP(U50,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W50" s="41"/>
-      <c r="X50" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W50,Services!$A$1:$B$45,2)),"",VLOOKUP(W50,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y50" s="41"/>
-      <c r="Z50" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y50,Services!$A$1:$B$45,2)),"",VLOOKUP(Y50,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA50" s="41"/>
-      <c r="AB50" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA50,Services!$A$1:$B$45,2)),"",VLOOKUP(AA50,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC50" s="41"/>
+      <c r="N50" s="1"/>
+      <c r="O50" s="1"/>
+      <c r="P50" s="41"/>
+      <c r="Q50" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P50,Services!$A$1:$B$45,2)),"",VLOOKUP(P50,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R50" s="41"/>
+      <c r="S50" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R50,Services!$A$1:$B$45,2)),"",VLOOKUP(R50,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T50" s="41"/>
+      <c r="U50" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T50,Services!$A$1:$B$45,2)),"",VLOOKUP(T50,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V50" s="41"/>
+      <c r="W50" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V50,Services!$A$1:$B$45,2)),"",VLOOKUP(V50,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X50" s="41"/>
+      <c r="Y50" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X50,Services!$A$1:$B$45,2)),"",VLOOKUP(X50,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z50" s="41"/>
+      <c r="AA50" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z50,Services!$A$1:$B$45,2)),"",VLOOKUP(Z50,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB50" s="41"/>
+      <c r="AC50" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB50,Services!$A$1:$B$45,2)),"",VLOOKUP(AB50,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD50" s="41"/>
+      <c r="AE50" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AD50,Services!$A$1:$B$45,2)),"",VLOOKUP(AD50,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AF50" s="41"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
@@ -11129,7 +11219,7 @@
           <x14:formula1>
             <xm:f>Services!$A$1:$A$43</xm:f>
           </x14:formula1>
-          <xm:sqref>Q2:Q50 S2:S50 U2:U50 W2:W50 Y2:Y50 AA2:AA50 M2:M50 O2:O50</xm:sqref>
+          <xm:sqref>T2:T50 V2:V50 X2:X50 Z2:Z50 AB2:AB50 AD2:AD50 P2:P50 R2:R50</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{69AD3E96-9986-4437-A6D2-54EE41465A4B}">
           <x14:formula1>
@@ -11147,13 +11237,13 @@
           <x14:formula1>
             <xm:f>Roles!$A$1:$A$2</xm:f>
           </x14:formula1>
-          <xm:sqref>K2:L50</xm:sqref>
+          <xm:sqref>K2:O50</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0B1666EF-45EA-466E-BF9B-CD6C235D8633}">
           <x14:formula1>
             <xm:f>Validations!$A$1:$A$2</xm:f>
           </x14:formula1>
-          <xm:sqref>AD2:AD50 AE2:AF5</xm:sqref>
+          <xm:sqref>M2:M50 N2:N5 O2:O5</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -11202,7 +11292,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="IrVQ7Ukz2v/R7gQxangUL5wAqS1715tiGhzT8zLeCz8UJwUIBrCLI/UycSYlC8mt/P4bgWL9vpSls59MeyEaVg==" saltValue="9syDTPxVg8TLEzOvGTicbQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -11584,7 +11673,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="aMZLA0VNhh5Onc5JvFgRcO+m2AuGfgKZ7BoJklGYjHaipO31AQ3xGW7Ut3i3WYaf9wFLoxFNYPTBp+0/KJwncA==" saltValue="2GsNMsCJLWlXXOIX1gAyDg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18816,7 +18904,6 @@
     <row r="741" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="742" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="m8UckgdD1dcYD9lqf4mZ6sweQUAjls9wUBQbAbH6Fx4sDdSYOTY5ss+Y9DW0iJlEs+St9Rf87Aa3SmKNJ6YBnQ==" saltValue="jfT1mkCRVBT5GRvlbF+nFg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <hyperlinks>
     <hyperlink ref="A287" r:id="rId1" display="https://courttribunalfinder.service.gov.uk/courts/sunderland-county-family-magistrates-and-tribunal-hearings" xr:uid="{E75D3469-3062-4D00-9760-56E3C0055DF4}"/>
   </hyperlinks>
@@ -18910,7 +18997,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="9Dzbl1Vp2as7XYFJXUh3e5BVC8sA06Mwnij3IjqsMXS9OIFgu8FBluC3Lbx7+HH6n1k9gv2FDDtFo6g8N0a+SA==" saltValue="2ONKPZCzYuddgylpf3RncA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -18949,7 +19035,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="K9Ci/eHmkmskFS0u1ZcnQkRZSqVBH/Kvod5Cg143QmMMqKBzxu71t7mKY0rKC7jAIRToE1wAYtCUnAacyc3hTg==" saltValue="vAGcL88qkz3LKuOeKothwQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -18975,7 +19060,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="D22dSHc3htXuo0x/4I3E9zXiFJcvy3Um+2pZMVdKjhStG73OU02OP04I/9LO7uth2Ls3E1T7wBkvo4tC4iIMtQ==" saltValue="zUVhzd2HkNeGZm+LUf4U+A==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Functional Tests and Excel File
</commit_message>
<xml_diff>
--- a/src/functionalTest/resources/Staff Data Upload with non idam roles.xlsx
+++ b/src/functionalTest/resources/Staff Data Upload with non idam roles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_2109032/RDCC4025/rd-caseworker-ref-api/src/functionalTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83AB114-2073-9D42-8C67-D85D8DBA340A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7677CDC5-5320-FC4A-8D44-B51F8C4BAA6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19520" activeTab="2" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19520" activeTab="7" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Guidance" sheetId="11" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1890" uniqueCount="1212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1898" uniqueCount="1220">
   <si>
     <t>Region</t>
   </si>
@@ -3680,6 +3680,30 @@
   </si>
   <si>
     <t>Service1</t>
+  </si>
+  <si>
+    <t>Hearing Centre Team Leader </t>
+  </si>
+  <si>
+    <t>Hearing Centre Administrator</t>
+  </si>
+  <si>
+    <t>Court Clerk</t>
+  </si>
+  <si>
+    <t>National Business Centre Team leader</t>
+  </si>
+  <si>
+    <t>National Business Centre Listing team</t>
+  </si>
+  <si>
+    <t>National Business Centre Payments team</t>
+  </si>
+  <si>
+    <t>CTSC team leader</t>
+  </si>
+  <si>
+    <t>CTSC Administrator</t>
   </si>
 </sst>
 </file>
@@ -7677,7 +7701,7 @@
   </sheetPr>
   <dimension ref="A1:AF50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
@@ -7816,15 +7840,15 @@
     <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" s="41" t="str">
         <f t="shared" ref="A2:B4" ca="1" si="0">CHAR(RANDBETWEEN(65,90))&amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122))</f>
-        <v>Amwj</v>
+        <v>Aumq</v>
       </c>
       <c r="B2" s="41" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Bpol</v>
+        <v>Lemt</v>
       </c>
       <c r="C2" s="42" t="str">
         <f ca="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
-        <v>CWR-func-test-user-2960309371@justice.gov.uk</v>
+        <v>CWR-func-test-user-6979207866@justice.gov.uk</v>
       </c>
       <c r="D2" s="41" t="s">
         <v>5</v>
@@ -7912,15 +7936,15 @@
     <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A3" s="41" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Ycbf</v>
+        <v>Qxde</v>
       </c>
       <c r="B3" s="41" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Ijej</v>
+        <v>Qwni</v>
       </c>
       <c r="C3" s="42" t="str">
         <f t="shared" ref="C3:C4" ca="1" si="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
-        <v>CWR-func-test-user-9466180198@justice.gov.uk</v>
+        <v>CWR-func-test-user-6392495206@justice.gov.uk</v>
       </c>
       <c r="D3" s="41" t="s">
         <v>6</v>
@@ -8004,15 +8028,15 @@
     <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" s="41" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Onax</v>
+        <v>Amys</v>
       </c>
       <c r="B4" s="41" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Zvyb</v>
+        <v>Tcpn</v>
       </c>
       <c r="C4" s="42" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>CWR-func-test-user-1300719135@justice.gov.uk</v>
+        <v>CWR-func-test-user-9095163193@justice.gov.uk</v>
       </c>
       <c r="D4" s="41" t="s">
         <v>9</v>
@@ -8104,7 +8128,7 @@
       </c>
       <c r="C5" s="42" t="str">
         <f ca="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
-        <v>CWR-func-test-user-3815393503@justice.gov.uk</v>
+        <v>CWR-func-test-user-5037109006@justice.gov.uk</v>
       </c>
       <c r="D5" s="41" t="s">
         <v>4</v>
@@ -19006,10 +19030,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -19032,6 +19056,70 @@
       </c>
       <c r="B2">
         <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>1212</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>1213</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>1214</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>1215</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>1216</v>
+      </c>
+      <c r="B7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>1217</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>1218</v>
+      </c>
+      <c r="B9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>1219</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RDCC-5182 fix for version compare in SRD file
</commit_message>
<xml_diff>
--- a/src/functionalTest/resources/Staff Data Upload with non idam roles.xlsx
+++ b/src/functionalTest/resources/Staff Data Upload with non idam roles.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_900458/Documents/HMCTS/rd-caseworker-ref-api/src/functionalTest/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_2088737/IdeaProjects/refdata_workspace/RDCC-5182/rd-caseworker-ref-api/src/functionalTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B34E4C3-6129-814A-B251-F532D50C9CF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2415966C-0EFC-894F-A10E-3F189EA59B7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" activeTab="2" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Guidance" sheetId="11" r:id="rId1"/>
-    <sheet name="Terminology" sheetId="12" r:id="rId2"/>
-    <sheet name="Staff Data" sheetId="1" r:id="rId3"/>
-    <sheet name="User Type" sheetId="9" r:id="rId4"/>
-    <sheet name="Services" sheetId="7" r:id="rId5"/>
-    <sheet name="Base Locations" sheetId="6" r:id="rId6"/>
-    <sheet name="Region" sheetId="3" r:id="rId7"/>
-    <sheet name="Roles" sheetId="4" r:id="rId8"/>
-    <sheet name="Validations" sheetId="10" r:id="rId9"/>
+    <sheet name="VERSION" sheetId="13" r:id="rId1"/>
+    <sheet name="Guidance" sheetId="11" r:id="rId2"/>
+    <sheet name="Terminology" sheetId="12" r:id="rId3"/>
+    <sheet name="Staff Data" sheetId="1" r:id="rId4"/>
+    <sheet name="User Type" sheetId="9" r:id="rId5"/>
+    <sheet name="Services" sheetId="7" r:id="rId6"/>
+    <sheet name="Base Locations" sheetId="6" r:id="rId7"/>
+    <sheet name="Region" sheetId="3" r:id="rId8"/>
+    <sheet name="Roles" sheetId="4" r:id="rId9"/>
+    <sheet name="Validations" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,11 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1903" uniqueCount="1226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1905" uniqueCount="1228">
   <si>
     <t>Region</t>
   </si>
@@ -3720,6 +3725,12 @@
   </si>
   <si>
     <t>Legal Caseworker</t>
+  </si>
+  <si>
+    <t>File version</t>
+  </si>
+  <si>
+    <t>vx.xx</t>
   </si>
 </sst>
 </file>
@@ -5008,6 +5019,54 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEBBE35D-861A-8A44-9C59-5FAA9F580C40}">
+  <dimension ref="A6:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>1226</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1227</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AF6684E-13C2-44AC-9BB0-45674920F5DD}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFDEFA66-BF37-4915-8EE3-57E3C043BC74}">
   <sheetPr>
     <tabColor theme="8" tint="0.39997558519241921"/>
@@ -7513,7 +7572,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBA3DD7B-56C8-415F-8BF5-7830E7EEFD36}">
   <sheetPr>
     <tabColor theme="8"/>
@@ -7712,14 +7771,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{535C96D2-347F-4382-9909-BFD50517035D}">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
   <dimension ref="A1:AF50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
@@ -7858,15 +7917,15 @@
     <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" s="40" t="str">
         <f t="shared" ref="A2:B4" ca="1" si="0">CHAR(RANDBETWEEN(65,90))&amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122))</f>
-        <v>Gngk</v>
+        <v>Ausz</v>
       </c>
       <c r="B2" s="40" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Qwuh</v>
+        <v>Ptcb</v>
       </c>
       <c r="C2" s="41" t="str">
         <f ca="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
-        <v>CWR-func-test-user-2130913005@justice.gov.uk</v>
+        <v>CWR-func-test-user-9618817367@justice.gov.uk</v>
       </c>
       <c r="D2" s="40" t="s">
         <v>5</v>
@@ -7954,15 +8013,15 @@
     <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A3" s="40" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Tiqo</v>
+        <v>Lgzl</v>
       </c>
       <c r="B3" s="40" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Mrbj</v>
+        <v>Csqs</v>
       </c>
       <c r="C3" s="41" t="str">
         <f t="shared" ref="C3:C4" ca="1" si="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
-        <v>CWR-func-test-user-2894529024@justice.gov.uk</v>
+        <v>CWR-func-test-user-9558622347@justice.gov.uk</v>
       </c>
       <c r="D3" s="40" t="s">
         <v>6</v>
@@ -8046,15 +8105,15 @@
     <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" s="40" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Iygs</v>
+        <v>Wqtw</v>
       </c>
       <c r="B4" s="40" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Ykwu</v>
+        <v>Nxgx</v>
       </c>
       <c r="C4" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>CWR-func-test-user-7740741483@justice.gov.uk</v>
+        <v>CWR-func-test-user-4966439786@justice.gov.uk</v>
       </c>
       <c r="D4" s="40" t="s">
         <v>9</v>
@@ -8146,7 +8205,7 @@
       </c>
       <c r="C5" s="41" t="str">
         <f ca="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
-        <v>CWR-func-test-user-5553785461@justice.gov.uk</v>
+        <v>CWR-func-test-user-3844732469@justice.gov.uk</v>
       </c>
       <c r="D5" s="40" t="s">
         <v>4</v>
@@ -11293,7 +11352,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55979B3E-2A8A-4780-BEB6-4F2717396A4D}">
   <sheetPr>
     <tabColor theme="7"/>
@@ -11338,7 +11397,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCA924CA-E283-4D75-8C37-FFE0D56B674F}">
   <sheetPr>
     <tabColor theme="7"/>
@@ -11720,7 +11779,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C18EAE82-4C6E-4D34-88FC-425D89B632D4}">
   <sheetPr>
     <tabColor theme="7"/>
@@ -18953,7 +19012,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9252D81-E1C7-47AA-BB50-43B308C890E9}">
   <sheetPr>
     <tabColor theme="7"/>
@@ -19043,7 +19102,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{175CCEB2-E456-408C-B252-200A77CE2E77}">
   <sheetPr>
     <tabColor theme="7"/>
@@ -19183,29 +19242,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AF6684E-13C2-44AC-9BB0-45674920F5DD}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>1112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
RDCC-5182 SRD file version validation changes
</commit_message>
<xml_diff>
--- a/src/functionalTest/resources/Staff Data Upload with non idam roles.xlsx
+++ b/src/functionalTest/resources/Staff Data Upload with non idam roles.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_900458/Documents/HMCTS/rd-caseworker-ref-api/src/functionalTest/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_2088737/IdeaProjects/refdata_workspace/RDCC-5182/rd-caseworker-ref-api/src/functionalTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B34E4C3-6129-814A-B251-F532D50C9CF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2415966C-0EFC-894F-A10E-3F189EA59B7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" activeTab="2" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Guidance" sheetId="11" r:id="rId1"/>
-    <sheet name="Terminology" sheetId="12" r:id="rId2"/>
-    <sheet name="Staff Data" sheetId="1" r:id="rId3"/>
-    <sheet name="User Type" sheetId="9" r:id="rId4"/>
-    <sheet name="Services" sheetId="7" r:id="rId5"/>
-    <sheet name="Base Locations" sheetId="6" r:id="rId6"/>
-    <sheet name="Region" sheetId="3" r:id="rId7"/>
-    <sheet name="Roles" sheetId="4" r:id="rId8"/>
-    <sheet name="Validations" sheetId="10" r:id="rId9"/>
+    <sheet name="VERSION" sheetId="13" r:id="rId1"/>
+    <sheet name="Guidance" sheetId="11" r:id="rId2"/>
+    <sheet name="Terminology" sheetId="12" r:id="rId3"/>
+    <sheet name="Staff Data" sheetId="1" r:id="rId4"/>
+    <sheet name="User Type" sheetId="9" r:id="rId5"/>
+    <sheet name="Services" sheetId="7" r:id="rId6"/>
+    <sheet name="Base Locations" sheetId="6" r:id="rId7"/>
+    <sheet name="Region" sheetId="3" r:id="rId8"/>
+    <sheet name="Roles" sheetId="4" r:id="rId9"/>
+    <sheet name="Validations" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,11 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1903" uniqueCount="1226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1905" uniqueCount="1228">
   <si>
     <t>Region</t>
   </si>
@@ -3720,6 +3725,12 @@
   </si>
   <si>
     <t>Legal Caseworker</t>
+  </si>
+  <si>
+    <t>File version</t>
+  </si>
+  <si>
+    <t>vx.xx</t>
   </si>
 </sst>
 </file>
@@ -5008,6 +5019,54 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEBBE35D-861A-8A44-9C59-5FAA9F580C40}">
+  <dimension ref="A6:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>1226</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1227</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AF6684E-13C2-44AC-9BB0-45674920F5DD}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFDEFA66-BF37-4915-8EE3-57E3C043BC74}">
   <sheetPr>
     <tabColor theme="8" tint="0.39997558519241921"/>
@@ -7513,7 +7572,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBA3DD7B-56C8-415F-8BF5-7830E7EEFD36}">
   <sheetPr>
     <tabColor theme="8"/>
@@ -7712,14 +7771,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{535C96D2-347F-4382-9909-BFD50517035D}">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
   <dimension ref="A1:AF50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
@@ -7858,15 +7917,15 @@
     <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" s="40" t="str">
         <f t="shared" ref="A2:B4" ca="1" si="0">CHAR(RANDBETWEEN(65,90))&amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122))</f>
-        <v>Gngk</v>
+        <v>Ausz</v>
       </c>
       <c r="B2" s="40" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Qwuh</v>
+        <v>Ptcb</v>
       </c>
       <c r="C2" s="41" t="str">
         <f ca="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
-        <v>CWR-func-test-user-2130913005@justice.gov.uk</v>
+        <v>CWR-func-test-user-9618817367@justice.gov.uk</v>
       </c>
       <c r="D2" s="40" t="s">
         <v>5</v>
@@ -7954,15 +8013,15 @@
     <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A3" s="40" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Tiqo</v>
+        <v>Lgzl</v>
       </c>
       <c r="B3" s="40" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Mrbj</v>
+        <v>Csqs</v>
       </c>
       <c r="C3" s="41" t="str">
         <f t="shared" ref="C3:C4" ca="1" si="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
-        <v>CWR-func-test-user-2894529024@justice.gov.uk</v>
+        <v>CWR-func-test-user-9558622347@justice.gov.uk</v>
       </c>
       <c r="D3" s="40" t="s">
         <v>6</v>
@@ -8046,15 +8105,15 @@
     <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" s="40" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Iygs</v>
+        <v>Wqtw</v>
       </c>
       <c r="B4" s="40" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Ykwu</v>
+        <v>Nxgx</v>
       </c>
       <c r="C4" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>CWR-func-test-user-7740741483@justice.gov.uk</v>
+        <v>CWR-func-test-user-4966439786@justice.gov.uk</v>
       </c>
       <c r="D4" s="40" t="s">
         <v>9</v>
@@ -8146,7 +8205,7 @@
       </c>
       <c r="C5" s="41" t="str">
         <f ca="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
-        <v>CWR-func-test-user-5553785461@justice.gov.uk</v>
+        <v>CWR-func-test-user-3844732469@justice.gov.uk</v>
       </c>
       <c r="D5" s="40" t="s">
         <v>4</v>
@@ -11293,7 +11352,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55979B3E-2A8A-4780-BEB6-4F2717396A4D}">
   <sheetPr>
     <tabColor theme="7"/>
@@ -11338,7 +11397,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCA924CA-E283-4D75-8C37-FFE0D56B674F}">
   <sheetPr>
     <tabColor theme="7"/>
@@ -11720,7 +11779,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C18EAE82-4C6E-4D34-88FC-425D89B632D4}">
   <sheetPr>
     <tabColor theme="7"/>
@@ -18953,7 +19012,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9252D81-E1C7-47AA-BB50-43B308C890E9}">
   <sheetPr>
     <tabColor theme="7"/>
@@ -19043,7 +19102,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{175CCEB2-E456-408C-B252-200A77CE2E77}">
   <sheetPr>
     <tabColor theme="7"/>
@@ -19183,29 +19242,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AF6684E-13C2-44AC-9BB0-45674920F5DD}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>1112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "RDCC-5182 fix for version compare in SRD file"
</commit_message>
<xml_diff>
--- a/src/functionalTest/resources/Staff Data Upload with non idam roles.xlsx
+++ b/src/functionalTest/resources/Staff Data Upload with non idam roles.xlsx
@@ -1,28 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_2088737/IdeaProjects/refdata_workspace/RDCC-5182/rd-caseworker-ref-api/src/functionalTest/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_900458/Documents/HMCTS/rd-caseworker-ref-api/src/functionalTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2415966C-0EFC-894F-A10E-3F189EA59B7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B34E4C3-6129-814A-B251-F532D50C9CF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" activeTab="2" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
   </bookViews>
   <sheets>
-    <sheet name="VERSION" sheetId="13" r:id="rId1"/>
-    <sheet name="Guidance" sheetId="11" r:id="rId2"/>
-    <sheet name="Terminology" sheetId="12" r:id="rId3"/>
-    <sheet name="Staff Data" sheetId="1" r:id="rId4"/>
-    <sheet name="User Type" sheetId="9" r:id="rId5"/>
-    <sheet name="Services" sheetId="7" r:id="rId6"/>
-    <sheet name="Base Locations" sheetId="6" r:id="rId7"/>
-    <sheet name="Region" sheetId="3" r:id="rId8"/>
-    <sheet name="Roles" sheetId="4" r:id="rId9"/>
-    <sheet name="Validations" sheetId="10" r:id="rId10"/>
+    <sheet name="Guidance" sheetId="11" r:id="rId1"/>
+    <sheet name="Terminology" sheetId="12" r:id="rId2"/>
+    <sheet name="Staff Data" sheetId="1" r:id="rId3"/>
+    <sheet name="User Type" sheetId="9" r:id="rId4"/>
+    <sheet name="Services" sheetId="7" r:id="rId5"/>
+    <sheet name="Base Locations" sheetId="6" r:id="rId6"/>
+    <sheet name="Region" sheetId="3" r:id="rId7"/>
+    <sheet name="Roles" sheetId="4" r:id="rId8"/>
+    <sheet name="Validations" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,11 +31,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -44,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1905" uniqueCount="1228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1903" uniqueCount="1226">
   <si>
     <t>Region</t>
   </si>
@@ -3725,12 +3720,6 @@
   </si>
   <si>
     <t>Legal Caseworker</t>
-  </si>
-  <si>
-    <t>File version</t>
-  </si>
-  <si>
-    <t>vx.xx</t>
   </si>
 </sst>
 </file>
@@ -5019,54 +5008,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEBBE35D-861A-8A44-9C59-5FAA9F580C40}">
-  <dimension ref="A6:B6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>1226</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1227</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AF6684E-13C2-44AC-9BB0-45674920F5DD}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>1112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFDEFA66-BF37-4915-8EE3-57E3C043BC74}">
   <sheetPr>
     <tabColor theme="8" tint="0.39997558519241921"/>
@@ -7572,7 +7513,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBA3DD7B-56C8-415F-8BF5-7830E7EEFD36}">
   <sheetPr>
     <tabColor theme="8"/>
@@ -7771,14 +7712,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{535C96D2-347F-4382-9909-BFD50517035D}">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
   <dimension ref="A1:AF50"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
@@ -7917,15 +7858,15 @@
     <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" s="40" t="str">
         <f t="shared" ref="A2:B4" ca="1" si="0">CHAR(RANDBETWEEN(65,90))&amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122))</f>
-        <v>Ausz</v>
+        <v>Gngk</v>
       </c>
       <c r="B2" s="40" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Ptcb</v>
+        <v>Qwuh</v>
       </c>
       <c r="C2" s="41" t="str">
         <f ca="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
-        <v>CWR-func-test-user-9618817367@justice.gov.uk</v>
+        <v>CWR-func-test-user-2130913005@justice.gov.uk</v>
       </c>
       <c r="D2" s="40" t="s">
         <v>5</v>
@@ -8013,15 +7954,15 @@
     <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A3" s="40" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Lgzl</v>
+        <v>Tiqo</v>
       </c>
       <c r="B3" s="40" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Csqs</v>
+        <v>Mrbj</v>
       </c>
       <c r="C3" s="41" t="str">
         <f t="shared" ref="C3:C4" ca="1" si="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
-        <v>CWR-func-test-user-9558622347@justice.gov.uk</v>
+        <v>CWR-func-test-user-2894529024@justice.gov.uk</v>
       </c>
       <c r="D3" s="40" t="s">
         <v>6</v>
@@ -8105,15 +8046,15 @@
     <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" s="40" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Wqtw</v>
+        <v>Iygs</v>
       </c>
       <c r="B4" s="40" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Nxgx</v>
+        <v>Ykwu</v>
       </c>
       <c r="C4" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>CWR-func-test-user-4966439786@justice.gov.uk</v>
+        <v>CWR-func-test-user-7740741483@justice.gov.uk</v>
       </c>
       <c r="D4" s="40" t="s">
         <v>9</v>
@@ -8205,7 +8146,7 @@
       </c>
       <c r="C5" s="41" t="str">
         <f ca="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
-        <v>CWR-func-test-user-3844732469@justice.gov.uk</v>
+        <v>CWR-func-test-user-5553785461@justice.gov.uk</v>
       </c>
       <c r="D5" s="40" t="s">
         <v>4</v>
@@ -11352,7 +11293,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55979B3E-2A8A-4780-BEB6-4F2717396A4D}">
   <sheetPr>
     <tabColor theme="7"/>
@@ -11397,7 +11338,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCA924CA-E283-4D75-8C37-FFE0D56B674F}">
   <sheetPr>
     <tabColor theme="7"/>
@@ -11779,7 +11720,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C18EAE82-4C6E-4D34-88FC-425D89B632D4}">
   <sheetPr>
     <tabColor theme="7"/>
@@ -19012,7 +18953,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9252D81-E1C7-47AA-BB50-43B308C890E9}">
   <sheetPr>
     <tabColor theme="7"/>
@@ -19102,7 +19043,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{175CCEB2-E456-408C-B252-200A77CE2E77}">
   <sheetPr>
     <tabColor theme="7"/>
@@ -19242,4 +19183,29 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AF6684E-13C2-44AC-9BB0-45674920F5DD}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Email Change in the XL sheet
</commit_message>
<xml_diff>
--- a/src/functionalTest/resources/Staff Data Upload with non idam roles.xlsx
+++ b/src/functionalTest/resources/Staff Data Upload with non idam roles.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vasthava/IdeaProjects/nayeem/rd-caseworker-ref-api/src/functionalTest/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hmcts/IdeaProjects/rd-caseworker/src/functionalTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CDB19A7-B044-E94B-BBA9-EA054B249D2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8990411D-2401-B64B-949F-B5467E15576C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="16440" activeTab="2" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="35840" windowHeight="21920" activeTab="2" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Guidance" sheetId="11" r:id="rId1"/>
@@ -3727,7 +3727,7 @@
     <t>Legal Caseworker</t>
   </si>
   <si>
-    <t>cwr-func-test-user</t>
+    <t>cwr-rd-func-test-user-only</t>
   </si>
 </sst>
 </file>
@@ -7725,7 +7725,7 @@
   <dimension ref="A1:AF50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7865,12 +7865,12 @@
         <v>1226</v>
       </c>
       <c r="B2" s="40" t="str">
-        <f t="shared" ref="A2:B4" ca="1" si="0">CHAR(RANDBETWEEN(65,90))&amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122))</f>
-        <v>Mnyd</v>
+        <f t="shared" ref="B2:B4" ca="1" si="0">CHAR(RANDBETWEEN(65,90))&amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122))</f>
+        <v>Fcub</v>
       </c>
       <c r="C2" s="40" t="str">
-        <f ca="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
-        <v>CWR-func-test-user-8122437074@justice.gov.uk</v>
+        <f ca="1">CONCATENATE("CWR-rd-func-test-user-only-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
+        <v>CWR-rd-func-test-user-only-5825268791@justice.gov.uk</v>
       </c>
       <c r="D2" s="40" t="s">
         <v>5</v>
@@ -7961,11 +7961,11 @@
       </c>
       <c r="B3" s="40" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Ugwt</v>
+        <v>Eqyq</v>
       </c>
       <c r="C3" s="40" t="str">
-        <f t="shared" ref="C3:C4" ca="1" si="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
-        <v>CWR-func-test-user-1327278331@justice.gov.uk</v>
+        <f t="shared" ref="C3:C5" ca="1" si="1">CONCATENATE("CWR-rd-func-test-user-only-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
+        <v>CWR-rd-func-test-user-only-7323661366@justice.gov.uk</v>
       </c>
       <c r="D3" s="40" t="s">
         <v>6</v>
@@ -8052,11 +8052,11 @@
       </c>
       <c r="B4" s="40" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Qynm</v>
+        <v>Nliz</v>
       </c>
       <c r="C4" s="40" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>CWR-func-test-user-2943169622@justice.gov.uk</v>
+        <v>CWR-rd-func-test-user-only-9068097730@justice.gov.uk</v>
       </c>
       <c r="D4" s="40" t="s">
         <v>9</v>
@@ -8147,8 +8147,8 @@
         <v>1191</v>
       </c>
       <c r="C5" s="40" t="str">
-        <f ca="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
-        <v>CWR-func-test-user-7234474505@justice.gov.uk</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>CWR-rd-func-test-user-only-5612018852@justice.gov.uk</v>
       </c>
       <c r="D5" s="40" t="s">
         <v>4</v>

</xml_diff>